<commit_message>
Update covid-19 contact forms to coalesce number properly
</commit_message>
<xml_diff>
--- a/config/covid-19/forms/contact/PLACE_TYPE-create.xlsx
+++ b/config/covid-19/forms/contact/PLACE_TYPE-create.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="survey" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="choices" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="settings" sheetId="3" r:id="rId6"/>
+    <sheet name="survey" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="choices" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="settings" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mjoid+fSX0Qkhf0uQyogBH92gIeJg=="/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="363">
   <si>
     <t>type</t>
   </si>
@@ -98,7 +95,7 @@
     <t>notes</t>
   </si>
   <si>
-    <t>begin group</t>
+    <t xml:space="preserve">begin group</t>
   </si>
   <si>
     <t>inputs</t>
@@ -116,19 +113,19 @@
     <t>contact_id</t>
   </si>
   <si>
-    <t>Contact ID of the logged in user</t>
+    <t xml:space="preserve">Contact ID of the logged in user</t>
   </si>
   <si>
     <t>facility_id</t>
   </si>
   <si>
-    <t>Place ID of the logged in user</t>
-  </si>
-  <si>
-    <t>Name of the logged in user</t>
-  </si>
-  <si>
-    <t>end group</t>
+    <t xml:space="preserve">Place ID of the logged in user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of the logged in user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end group</t>
   </si>
   <si>
     <t>init</t>
@@ -137,28 +134,28 @@
     <t>field-list</t>
   </si>
   <si>
-    <t>select_one contact</t>
+    <t xml:space="preserve">select_one contact</t>
   </si>
   <si>
     <t>create_new_person</t>
   </si>
   <si>
-    <t>Set the primary contact</t>
-  </si>
-  <si>
-    <t>प्राथमिक कॉंटॅक्ट चुनें</t>
-  </si>
-  <si>
-    <t>Ditetapkan Sebagai Kontak Utama</t>
-  </si>
-  <si>
-    <t>Weka mwasiliwa mkuu</t>
-  </si>
-  <si>
-    <t>प्राथमिक सम्पर्क व्यक्ति</t>
-  </si>
-  <si>
-    <t>Contact primaire</t>
+    <t xml:space="preserve">Set the primary contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">प्राथमिक कॉंटॅक्ट चुनें</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ditetapkan Sebagai Kontak Utama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weka mwasiliwa mkuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">प्राथमिक सम्पर्क व्यक्ति</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact primaire</t>
   </si>
   <si>
     <t>yes</t>
@@ -173,19 +170,19 @@
     <t>select_person</t>
   </si>
   <si>
-    <t>Select the primary contact</t>
-  </si>
-  <si>
-    <t>Pilih Kontak Utama</t>
-  </si>
-  <si>
-    <t>Chagua Mwasiliwa mkuu</t>
-  </si>
-  <si>
-    <t>प्राथमिक सम्पर्क व्यक्ति छान्नुहोस्</t>
-  </si>
-  <si>
-    <t>Choisisser le contact primaire</t>
+    <t xml:space="preserve">Select the primary contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pilih Kontak Utama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chagua Mwasiliwa mkuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">प्राथमिक सम्पर्क व्यक्ति छान्नुहोस्</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choisisser le contact primaire</t>
   </si>
   <si>
     <t>selected(${create_new_person},'old_person')</t>
@@ -203,10 +200,10 @@
     <t>contact_name</t>
   </si>
   <si>
-    <t>coalesce(../../contact/name, ../name)</t>
-  </si>
-  <si>
-    <t>select_one translate_name_label</t>
+    <t xml:space="preserve">coalesce(../../contact/name, ../name)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one translate_name_label</t>
   </si>
   <si>
     <t>custom_place_name_label_translator</t>
@@ -230,34 +227,34 @@
     <t>${custom_place_name_label}</t>
   </si>
   <si>
-    <t>selected(${create_new_person},'none') or selected(${is_name_generated}, 'false')  or selected(${is_name_generated}, 'no')</t>
-  </si>
-  <si>
-    <t>Standalone question only if no contact is selected, so show label accordingly</t>
-  </si>
-  <si>
-    <t>select_one place_type</t>
+    <t xml:space="preserve">selected(${create_new_person},'none') or selected(${is_name_generated}, 'false')  or selected(${is_name_generated}, 'no')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standalone question only if no contact is selected, so show label accordingly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one place_type</t>
   </si>
   <si>
     <t>place_type</t>
   </si>
   <si>
-    <t>Enter the name of this place</t>
-  </si>
-  <si>
-    <t>इस स्थान का नाम दर्ज करें</t>
-  </si>
-  <si>
-    <t>Masukkan nama tempat ini</t>
-  </si>
-  <si>
-    <t>Jaza jina la eneo hii</t>
-  </si>
-  <si>
-    <t>यस स्थानको नाम लेख्नुहोस्</t>
-  </si>
-  <si>
-    <t>Nom de l'endroit</t>
+    <t xml:space="preserve">Enter the name of this place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">इस स्थान का नाम दर्ज करें</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masukkan nama tempat ini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jaza jina la eneo hii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">यस स्थानको नाम लेख्नुहोस्</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nom de l'endroit</t>
   </si>
   <si>
     <t>PLACE_TYPE</t>
@@ -269,7 +266,7 @@
     <t>jr:choice-name(${place_type},'${place_type}')</t>
   </si>
   <si>
-    <t>select_one generated_name</t>
+    <t xml:space="preserve">select_one generated_name</t>
   </si>
   <si>
     <t>generated_name</t>
@@ -284,19 +281,19 @@
     <t>contact</t>
   </si>
   <si>
-    <t>New person</t>
-  </si>
-  <si>
-    <t>नया व्यक्ति</t>
-  </si>
-  <si>
-    <t>Orang Baru</t>
-  </si>
-  <si>
-    <t>Mtu Mpya</t>
-  </si>
-  <si>
-    <t>Nouvelle personne</t>
+    <t xml:space="preserve">New person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">नया व्यक्ति</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orang Baru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mtu Mpya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nouvelle personne</t>
   </si>
   <si>
     <t>selected(${create_new_person},'new_person')</t>
@@ -314,7 +311,7 @@
     <t>first_name</t>
   </si>
   <si>
-    <t>First name</t>
+    <t xml:space="preserve">First name</t>
   </si>
   <si>
     <t>last_name</t>
@@ -323,7 +320,7 @@
     <t xml:space="preserve">Last name </t>
   </si>
   <si>
-    <t>concat(${first_name}, ' ', ${last_name})</t>
+    <t xml:space="preserve">concat(${first_name}, ' ', ${last_name})</t>
   </si>
   <si>
     <t>date_of_birth</t>
@@ -353,13 +350,13 @@
     <t>not(selected(../dob_method,'approx'))</t>
   </si>
   <si>
-    <t>floor(decimal-date-time(.)) &lt;= floor(decimal-date-time(today()))</t>
-  </si>
-  <si>
-    <t>Date must be before today</t>
-  </si>
-  <si>
-    <t>Date of Birth</t>
+    <t xml:space="preserve">floor(decimal-date-time(.)) &lt;= floor(decimal-date-time(today()))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date must be before today</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of Birth</t>
   </si>
   <si>
     <t>note</t>
@@ -383,10 +380,10 @@
     <t>Years</t>
   </si>
   <si>
-    <t>. &gt;= 0 and . &lt;= 130</t>
-  </si>
-  <si>
-    <t>Age must be between 0 and 130</t>
+    <t xml:space="preserve">. &gt;= 0 and . &lt;= 130</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age must be between 0 and 130</t>
   </si>
   <si>
     <t>age_months</t>
@@ -395,13 +392,13 @@
     <t>Months</t>
   </si>
   <si>
-    <t>. &gt;= 0 and . &lt;= 11</t>
-  </si>
-  <si>
-    <t>Months must between 0 and 11</t>
-  </si>
-  <si>
-    <t>select_multiple select_dob_method</t>
+    <t xml:space="preserve">. &gt;= 0 and . &lt;= 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Months must between 0 and 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_multiple select_dob_method</t>
   </si>
   <si>
     <t>dob_method</t>
@@ -416,13 +413,13 @@
     <t>ephemeral_months</t>
   </si>
   <si>
-    <t>if(format-date-time(today(),"%m") - ../age_months &lt; 0, format-date-time(today(),"%m") - ../age_months + 12, format-date-time(today(),"%m") - ../age_months)</t>
+    <t xml:space="preserve">if(format-date-time(today(),"%m") - coalesce(../age_months, 0) &lt; 0, format-date-time(today(),"%m") - coalesce(../age_months, 0) + 12, format-date-time(today(),"%m") - coalesce(../age_months, 0))</t>
   </si>
   <si>
     <t>ephemeral_years</t>
   </si>
   <si>
-    <t>if(format-date-time(today(),"%m") - ../age_months &lt; 0, format-date-time(today(),"%Y") - ../age_years - 1, format-date-time(today(),"%Y") -../age_years)</t>
+    <t xml:space="preserve">if(format-date-time(today(),"%m") - coalesce(../age_months, 0) &lt; 0, format-date-time(today(),"%Y") - ../age_years - 1, format-date-time(today(),"%Y") -../age_years)</t>
   </si>
   <si>
     <t>dob_approx</t>
@@ -431,13 +428,13 @@
     <t>DOB</t>
   </si>
   <si>
-    <t>concat(string(${ephemeral_years}),'-',if(${ephemeral_months}&lt;10, concat('0',string(${ephemeral_months})), ${ephemeral_months}),'-',string(format-date-time(today(), "%d")))</t>
+    <t xml:space="preserve">concat(string(${ephemeral_years}),'-',if(${ephemeral_months}&lt;10, concat('0',string(${ephemeral_months})), ${ephemeral_months}),'-',string(format-date-time(today(), "%d")))</t>
   </si>
   <si>
     <t>dob_raw</t>
   </si>
   <si>
-    <t>if(not(selected( ../dob_method,'approx')), 
+    <t xml:space="preserve">if(not(selected( ../dob_method,'approx')), 
 ../dob_calendar,
 ../dob_approx)</t>
   </si>
@@ -445,7 +442,7 @@
     <t>dob_iso</t>
   </si>
   <si>
-    <t>Date of birth</t>
+    <t xml:space="preserve">Date of birth</t>
   </si>
   <si>
     <t>format-date-time(../dob_raw,"%Y-%m-%d")</t>
@@ -454,7 +451,7 @@
     <t>dob_debug</t>
   </si>
   <si>
-    <t>Months: ${ephemeral_months}
+    <t xml:space="preserve">Months: ${ephemeral_months}
 Year: ${ephemeral_years}
 DOB Approx: ${dob_approx}
 DOB Calendar: ${dob_calendar}
@@ -467,49 +464,49 @@
     <t>phone</t>
   </si>
   <si>
-    <t>Phone number</t>
-  </si>
-  <si>
-    <t>फोन नंबर</t>
-  </si>
-  <si>
-    <t>Nomor Telepon</t>
-  </si>
-  <si>
-    <t>Namba ya Simi</t>
-  </si>
-  <si>
-    <t>फाेन नम्बर</t>
+    <t xml:space="preserve">Phone number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">फोन नंबर</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nomor Telepon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namba ya Simi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">फाेन नम्बर</t>
   </si>
   <si>
     <t>Téléphone</t>
   </si>
   <si>
-    <t>Please enter a valid local number, or use the standard international format, which includes a plus sign (+) and country code. For example: +13125551211</t>
+    <t xml:space="preserve">Please enter a valid local number, or use the standard international format, which includes a plus sign (+) and country code. For example: +13125551211</t>
   </si>
   <si>
     <t>phone_alternate</t>
   </si>
   <si>
-    <t>Alternate phone number</t>
-  </si>
-  <si>
-    <t>अन्य फोन नंबर</t>
-  </si>
-  <si>
-    <t>Nomor Telepon Alternatif</t>
+    <t xml:space="preserve">Alternate phone number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">अन्य फोन नंबर</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nomor Telepon Alternatif</t>
   </si>
   <si>
     <t xml:space="preserve">Namba Ya </t>
   </si>
   <si>
-    <t>बैकल्पिक फाेन नम्बर</t>
-  </si>
-  <si>
-    <t>Téléphone alternatif</t>
-  </si>
-  <si>
-    <t>select_one male_female</t>
+    <t xml:space="preserve">बैकल्पिक फाेन नम्बर</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Téléphone alternatif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one male_female</t>
   </si>
   <si>
     <t>sex</t>
@@ -521,7 +518,7 @@
     <t>लिंग</t>
   </si>
   <si>
-    <t>Jenis kelamin</t>
+    <t xml:space="preserve">Jenis kelamin</t>
   </si>
   <si>
     <t>Jinsia</t>
@@ -536,7 +533,7 @@
     <t>Address</t>
   </si>
   <si>
-    <t>select_one roles</t>
+    <t xml:space="preserve">select_one roles</t>
   </si>
   <si>
     <t>role</t>
@@ -551,7 +548,7 @@
     <t>Peran</t>
   </si>
   <si>
-    <t>Namba ya simu Nyingine</t>
+    <t xml:space="preserve">Namba ya simu Nyingine</t>
   </si>
   <si>
     <t>भुमिका</t>
@@ -563,46 +560,46 @@
     <t>role_other</t>
   </si>
   <si>
-    <t>Specify other</t>
-  </si>
-  <si>
-    <t>अन्य का उल्‍लेख करें</t>
-  </si>
-  <si>
-    <t>Tentukan lainnya</t>
-  </si>
-  <si>
-    <t>Fafanua vingine</t>
-  </si>
-  <si>
-    <t>अन्य उल्लेख गर्नुहोस्</t>
+    <t xml:space="preserve">Specify other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">अन्य का उल्‍लेख करें</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tentukan lainnya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fafanua vingine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">अन्य उल्लेख गर्नुहोस्</t>
   </si>
   <si>
     <t>Specifier</t>
   </si>
   <si>
-    <t>selected( ${role},'other')</t>
+    <t xml:space="preserve">selected( ${role},'other')</t>
   </si>
   <si>
     <t>external_id</t>
   </si>
   <si>
-    <t>External ID</t>
-  </si>
-  <si>
-    <t>बाहरी ID</t>
-  </si>
-  <si>
-    <t>Eksternal ID</t>
-  </si>
-  <si>
-    <t>Kitambulisho cha nje</t>
-  </si>
-  <si>
-    <t>बाहिरि ID</t>
-  </si>
-  <si>
-    <t>Identifiant externe</t>
+    <t xml:space="preserve">External ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">बाहरी ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eksternal ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kitambulisho cha nje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">बाहिरि ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifiant externe</t>
   </si>
   <si>
     <t>Notes</t>
@@ -644,28 +641,28 @@
     <t>../../../inputs/user/facility_id</t>
   </si>
   <si>
-    <t>select_one yes_no_generated_name</t>
+    <t xml:space="preserve">select_one yes_no_generated_name</t>
   </si>
   <si>
     <t>is_name_generated</t>
   </si>
   <si>
-    <t>Would you like to name the place after the primary contact: "${generated_name_translation}"?</t>
-  </si>
-  <si>
-    <t>क्या आप इस स्थान को प्राथमिक कॉंटॅक्ट का नाम देना चाहेंगे?: ${generated_name_translation}</t>
-  </si>
-  <si>
-    <t>Apakah Anda ingin nama tempat setelah kontak utama: "${generated_name_translation}"?</t>
-  </si>
-  <si>
-    <t>Je, Ungependa kuita eneo hii kama mwasilishi mkuu wa eneo hii? "${generated_name_translation}"?</t>
-  </si>
-  <si>
-    <t>के तपाइ यस स्थानकाे प्राथमिक सम्पर्क नाम दिन चाहानु हुन्छ?:${generated_name_translation}</t>
-  </si>
-  <si>
-    <t>Voulez-vous nommer l'endroit: "${generated_name_translation}"?</t>
+    <t xml:space="preserve">Would you like to name the place after the primary contact: "${generated_name_translation}"?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">क्या आप इस स्थान को प्राथमिक कॉंटॅक्ट का नाम देना चाहेंगे?: ${generated_name_translation}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apakah Anda ingin nama tempat setelah kontak utama: "${generated_name_translation}"?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je, Ungependa kuita eneo hii kama mwasilishi mkuu wa eneo hii? "${generated_name_translation}"?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">के तपाइ यस स्थानकाे प्राथमिक सम्पर्क नाम दिन चाहानु हुन्छ?:${generated_name_translation}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voulez-vous nommer l'endroit: "${generated_name_translation}"?</t>
   </si>
   <si>
     <t>not(selected(${create_new_person},'none'))</t>
@@ -689,19 +686,19 @@
     <t>Nom</t>
   </si>
   <si>
-    <t>if( ( selected(${is_name_generated}, 'true') or selected(${is_name_generated}, 'yes') ), ${generated_name_translation}, ${custom_place_name})</t>
-  </si>
-  <si>
-    <t>Namba ya nje</t>
-  </si>
-  <si>
-    <t>if(selected(${create_new_person},'none'), "", coalesce(${select_person},"NEW"))</t>
+    <t xml:space="preserve">if( ( selected(${is_name_generated}, 'true') or selected(${is_name_generated}, 'yes') ), ${generated_name_translation}, ${custom_place_name})</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namba ya nje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if(selected(${create_new_person},'none'), "", coalesce(${select_person},"NEW"))</t>
   </si>
   <si>
     <t>geolocation</t>
   </si>
   <si>
-    <t>concat(../../inputs/meta/location/lat, concat(' ', ../../inputs/meta/location/long))</t>
+    <t xml:space="preserve">concat(../../inputs/meta/location/lat, concat(' ', ../../inputs/meta/location/long))</t>
   </si>
   <si>
     <t>list_name</t>
@@ -797,64 +794,64 @@
     <t>new_person</t>
   </si>
   <si>
-    <t>Create a new person</t>
-  </si>
-  <si>
-    <t>एक नया व्यक्ति बनाएं</t>
-  </si>
-  <si>
-    <t>Buat orang baru</t>
-  </si>
-  <si>
-    <t>Ongeza mtumizi mpya</t>
-  </si>
-  <si>
-    <t>एक नया व्यक्ति बनाउनुस</t>
-  </si>
-  <si>
-    <t>Créer une nouvelle personne</t>
+    <t xml:space="preserve">Create a new person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">एक नया व्यक्ति बनाएं</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buat orang baru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ongeza mtumizi mpya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">एक नया व्यक्ति बनाउनुस</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer une nouvelle personne</t>
   </si>
   <si>
     <t>old_person</t>
   </si>
   <si>
-    <t>Select an existing person</t>
-  </si>
-  <si>
-    <t>मौजूदा व्यक्ति चुनें</t>
-  </si>
-  <si>
-    <t>Pilih orang yang ada</t>
-  </si>
-  <si>
-    <t>Chagua mtumizi aliyesajlishwa apo awali</t>
-  </si>
-  <si>
-    <t>व्यक्ति छान्नुहोस्</t>
-  </si>
-  <si>
-    <t>Selectiionner une personne existant</t>
+    <t xml:space="preserve">Select an existing person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">मौजूदा व्यक्ति चुनें</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pilih orang yang ada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chagua mtumizi aliyesajlishwa apo awali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">व्यक्ति छान्नुहोस्</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selectiionner une personne existant</t>
   </si>
   <si>
     <t>none</t>
   </si>
   <si>
-    <t>Skip this step</t>
-  </si>
-  <si>
-    <t>इस स्टेप को छोड़ दें</t>
-  </si>
-  <si>
-    <t>Lewati langkah ini</t>
-  </si>
-  <si>
-    <t>Ruka hatua ii</t>
+    <t xml:space="preserve">Skip this step</t>
+  </si>
+  <si>
+    <t xml:space="preserve">इस स्टेप को छोड़ दें</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lewati langkah ini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruka hatua ii</t>
   </si>
   <si>
     <t xml:space="preserve">एख </t>
   </si>
   <si>
-    <t>Sauter cette section</t>
+    <t xml:space="preserve">Sauter cette section</t>
   </si>
   <si>
     <t>select_dob_method</t>
@@ -863,7 +860,7 @@
     <t>approx</t>
   </si>
   <si>
-    <t>Date of birth unknown</t>
+    <t xml:space="preserve">Date of birth unknown</t>
   </si>
   <si>
     <t>roles</t>
@@ -875,16 +872,16 @@
     <t>CHW</t>
   </si>
   <si>
-    <t>सामुदायिक स्वास्थ्य कर्मी</t>
+    <t xml:space="preserve">सामुदायिक स्वास्थ्य कर्मी</t>
   </si>
   <si>
     <t>Kader</t>
   </si>
   <si>
-    <t>Mhudumu wa afya</t>
-  </si>
-  <si>
-    <t>महिला स्वास्थ्य स्वयम् सेविका</t>
+    <t xml:space="preserve">Mhudumu wa afya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">महिला स्वास्थ्य स्वयम् सेविका</t>
   </si>
   <si>
     <t>ASC</t>
@@ -893,22 +890,22 @@
     <t>chw_supervisor</t>
   </si>
   <si>
-    <t>CHW Supervisor</t>
-  </si>
-  <si>
-    <t>सामुदायिक स्वास्थ्य कर्मी के मैनेजर</t>
-  </si>
-  <si>
-    <t>Kader Pengawas</t>
-  </si>
-  <si>
-    <t>Mkuu wa wahudumu wa afya</t>
-  </si>
-  <si>
-    <t>महिला स्वास्थ्य स्वयम् सेविकाको सुपरभाइजर</t>
-  </si>
-  <si>
-    <t>Superviseur ASC</t>
+    <t xml:space="preserve">CHW Supervisor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">सामुदायिक स्वास्थ्य कर्मी के मैनेजर</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kader Pengawas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mkuu wa wahudumu wa afya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">महिला स्वास्थ्य स्वयम् सेविकाको सुपरभाइजर</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Superviseur ASC</t>
   </si>
   <si>
     <t>patient</t>
@@ -953,28 +950,28 @@
     <t>हो</t>
   </si>
   <si>
-    <t>No, I want to name it manually</t>
-  </si>
-  <si>
-    <t>नहीं, मैं इसे मैन्युअल रूप से नाम देना चाहता हूं</t>
-  </si>
-  <si>
-    <t>Tidak, saya ingin nama itu secara manual</t>
-  </si>
-  <si>
-    <t>Hapana, ningependa kuijaza mwenyewe</t>
-  </si>
-  <si>
-    <t>होइन, म आफैँ नाम दिन चाहन्छु</t>
-  </si>
-  <si>
-    <t>Non, je veux nommer ça manuellement</t>
+    <t xml:space="preserve">No, I want to name it manually</t>
+  </si>
+  <si>
+    <t xml:space="preserve">नहीं, मैं इसे मैन्युअल रूप से नाम देना चाहता हूं</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tidak, saya ingin nama itu secara manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hapana, ningependa kuijaza mwenyewe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">होइन, म आफैँ नाम दिन चाहन्छु</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non, je veux nommer ça manuellement</t>
   </si>
   <si>
     <t>district_hospital</t>
   </si>
   <si>
-    <t>Health Facility</t>
+    <t xml:space="preserve">Health Facility</t>
   </si>
   <si>
     <t>ज़िला</t>
@@ -998,19 +995,19 @@
     <t>Area</t>
   </si>
   <si>
-    <t>स्वास्थ्य केंद्र</t>
-  </si>
-  <si>
-    <t>Fasilitas Kesehatan</t>
-  </si>
-  <si>
-    <t>Kituo cha afya</t>
-  </si>
-  <si>
-    <t>स्वास्थ्य केन्द्र</t>
-  </si>
-  <si>
-    <t>Centre de santé</t>
+    <t xml:space="preserve">स्वास्थ्य केंद्र</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fasilitas Kesehatan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kituo cha afya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">स्वास्थ्य केन्द्र</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centre de santé</t>
   </si>
   <si>
     <t>clinic</t>
@@ -1031,58 +1028,58 @@
     <t>Zone</t>
   </si>
   <si>
-    <t>${contact_name}'s Health Facility</t>
-  </si>
-  <si>
-    <t>${contact_name} का ज़िला</t>
+    <t xml:space="preserve">${contact_name}'s Health Facility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${contact_name} का ज़िला</t>
   </si>
   <si>
     <t xml:space="preserve">Kabupaten ${contact_name} </t>
   </si>
   <si>
-    <t>WIlaya ya  ${contact_name}</t>
+    <t xml:space="preserve">WIlaya ya  ${contact_name}</t>
   </si>
   <si>
     <t xml:space="preserve">${contact_name}को जिल्ला </t>
   </si>
   <si>
-    <t>District de ${contact_name}</t>
-  </si>
-  <si>
-    <t>${contact_name}'s Area</t>
-  </si>
-  <si>
-    <t>${contact_name} का स्वास्थ्य केंद्र</t>
+    <t xml:space="preserve">District de ${contact_name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${contact_name}'s Area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${contact_name} का स्वास्थ्य केंद्र</t>
   </si>
   <si>
     <t xml:space="preserve">Fasilitas Kesehatan ${contact_name} </t>
   </si>
   <si>
-    <t>Kituo cha afya cha  ${contact_name}</t>
-  </si>
-  <si>
-    <t>${contact_name}को स्वास्थ्य केन्द्र</t>
-  </si>
-  <si>
-    <t>Centre de santé de ${contact_name}</t>
-  </si>
-  <si>
-    <t>${contact_name}'s Household</t>
-  </si>
-  <si>
-    <t>${contact_name} का क्षेत्र</t>
+    <t xml:space="preserve">Kituo cha afya cha  ${contact_name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${contact_name}को स्वास्थ्य केन्द्र</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centre de santé de ${contact_name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${contact_name}'s Household</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${contact_name} का क्षेत्र</t>
   </si>
   <si>
     <t xml:space="preserve">Daerah ${contact_name} </t>
   </si>
   <si>
-    <t>Eneo ya  ${contact_name}</t>
-  </si>
-  <si>
-    <t>${contact_name}को क्षेत्र</t>
-  </si>
-  <si>
-    <t>Zone de ${contact_name}</t>
+    <t xml:space="preserve">Eneo ya  ${contact_name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${contact_name}को क्षेत्र</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone de ${contact_name}</t>
   </si>
   <si>
     <t>translate_name_label</t>
@@ -1103,7 +1100,7 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>New PLACE_NAME</t>
+    <t xml:space="preserve">New PLACE_NAME</t>
   </si>
   <si>
     <t>contact:PLACE_TYPE:create</t>
@@ -1118,32 +1115,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <color indexed="64"/>
+      <sz val="11.000000"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b/>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <color indexed="64"/>
+      <sz val="11.000000"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <name val="Calibri"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="11.000000"/>
     </font>
     <font>
-      <sz val="11.0"/>
       <name val="Calibri"/>
+      <sz val="11.000000"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
+      <color indexed="64"/>
+      <sz val="11.000000"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1151,7 +1148,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1209,169 +1206,388 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor indexed="65"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
-    <border/>
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
   <cellXfs count="41">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf fontId="1" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf fontId="1" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="1" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="1" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="1" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf fontId="2" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="2" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf fontId="3" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="3" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="2" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="2" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="2" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="4" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="8" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="9" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf fontId="0" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="10" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="10" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="11" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1428,7 +1644,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1454,7 +1670,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1506,16 +1722,28 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1531,7 +1759,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1561,49 +1789,49 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
-    <pageSetUpPr/>
+    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2.0" ySplit="1.0" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="C1" sqref="C1" pane="topRight"/>
-      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
-      <selection activeCell="C2" sqref="C2" pane="bottomRight"/>
+    <sheetView workbookViewId="0" zoomScale="100">
+      <pane activePane="bottomRight" state="frozen" topLeftCell="C2" xSplit="2" ySplit="1"/>
+      <selection activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="34.0"/>
-    <col customWidth="1" min="2" max="2" width="26.0"/>
-    <col customWidth="1" min="3" max="3" width="47.86"/>
+    <col customWidth="1" min="1" max="1" width="34"/>
+    <col customWidth="1" min="2" max="2" width="26"/>
+    <col customWidth="1" min="3" max="3" width="47.859999999999999"/>
     <col customWidth="1" hidden="1" min="4" max="4" width="33.43"/>
     <col customWidth="1" hidden="1" min="5" max="5" width="27.43"/>
-    <col customWidth="1" hidden="1" min="6" max="6" width="37.29"/>
-    <col customWidth="1" hidden="1" min="7" max="7" width="31.29"/>
-    <col customWidth="1" hidden="1" min="8" max="8" width="8.14"/>
-    <col customWidth="1" hidden="1" min="9" max="9" width="16.71"/>
-    <col customWidth="1" min="10" max="10" width="8.14"/>
+    <col customWidth="1" hidden="1" min="6" max="6" width="37.289999999999999"/>
+    <col customWidth="1" hidden="1" min="7" max="7" width="31.289999999999999"/>
+    <col customWidth="1" hidden="1" min="8" max="8" width="8.1400000000000006"/>
+    <col customWidth="1" hidden="1" min="9" max="9" width="16.710000000000001"/>
+    <col customWidth="1" min="10" max="10" width="8.1400000000000006"/>
     <col customWidth="1" min="11" max="11" width="51.43"/>
-    <col customWidth="1" min="12" max="13" width="10.71"/>
-    <col customWidth="1" min="14" max="14" width="25.29"/>
-    <col customWidth="1" min="15" max="15" width="46.29"/>
-    <col customWidth="1" min="16" max="16" width="68.86"/>
-    <col customWidth="1" min="17" max="17" width="9.43"/>
+    <col customWidth="1" min="12" max="13" width="10.710000000000001"/>
+    <col customWidth="1" min="14" max="14" width="25.289999999999999"/>
+    <col customWidth="1" min="15" max="15" width="46.289999999999999"/>
+    <col customWidth="1" min="16" max="16" width="68.859999999999999"/>
+    <col customWidth="1" min="17" max="17" width="9.4299999999999997"/>
     <col customWidth="1" min="18" max="18" width="33.43"/>
-    <col customWidth="1" min="19" max="19" width="36.29"/>
+    <col customWidth="1" min="19" max="19" width="36.289999999999999"/>
     <col customWidth="1" min="20" max="23" width="13.57"/>
     <col customWidth="1" min="24" max="24" width="7.71"/>
-    <col customWidth="1" min="25" max="25" width="8.71"/>
-    <col customWidth="1" min="26" max="26" width="35.86"/>
+    <col customWidth="1" min="25" max="25" width="8.7100000000000009"/>
+    <col customWidth="1" min="26" max="26" width="35.859999999999999"/>
     <col customWidth="1" min="27" max="36" width="7.71"/>
-    <col customWidth="1" min="37" max="38" width="15.14"/>
-    <col customWidth="1" min="39" max="44" width="17.29"/>
+    <col customWidth="1" min="37" max="38" width="15.140000000000001"/>
+    <col customWidth="1" min="39" max="44" width="17.289999999999999"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -2224,7 +2452,7 @@
       <c r="B11" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="16" t="s">
         <v>41</v>
       </c>
       <c r="D11" s="16" t="s">
@@ -2290,7 +2518,7 @@
       <c r="B12" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="16" t="s">
         <v>51</v>
       </c>
       <c r="D12" s="16" t="s">
@@ -2435,7 +2663,7 @@
       <c r="M14" s="16"/>
       <c r="N14" s="16"/>
       <c r="O14" s="16"/>
-      <c r="P14" s="19" t="s">
+      <c r="P14" s="18" t="s">
         <v>61</v>
       </c>
       <c r="Q14" s="16"/>
@@ -2477,7 +2705,7 @@
       <c r="C15" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="18" t="s">
         <v>28</v>
       </c>
       <c r="E15" s="16" t="s">
@@ -2543,7 +2771,7 @@
         <v>66</v>
       </c>
       <c r="C16" s="16"/>
-      <c r="D16" s="19"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
@@ -2554,8 +2782,8 @@
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19" t="s">
+      <c r="O16" s="18"/>
+      <c r="P16" s="18" t="s">
         <v>67</v>
       </c>
       <c r="Q16" s="16"/>
@@ -2689,7 +2917,7 @@
       <c r="M18" s="16"/>
       <c r="N18" s="16"/>
       <c r="O18" s="16"/>
-      <c r="P18" s="19"/>
+      <c r="P18" s="18"/>
       <c r="Q18" s="16"/>
       <c r="R18" s="16"/>
       <c r="S18" s="16"/>
@@ -2698,7 +2926,7 @@
       <c r="V18" s="16"/>
       <c r="W18" s="16"/>
       <c r="X18" s="16"/>
-      <c r="Y18" s="19" t="s">
+      <c r="Y18" s="18" t="s">
         <v>80</v>
       </c>
       <c r="Z18" s="16"/>
@@ -2741,7 +2969,7 @@
       <c r="M19" s="16"/>
       <c r="N19" s="16"/>
       <c r="O19" s="16"/>
-      <c r="P19" s="19" t="s">
+      <c r="P19" s="18" t="s">
         <v>82</v>
       </c>
       <c r="Q19" s="16"/>
@@ -2816,7 +3044,7 @@
       <c r="V20" s="16"/>
       <c r="W20" s="16"/>
       <c r="X20" s="16"/>
-      <c r="Y20" s="19" t="s">
+      <c r="Y20" s="18" t="s">
         <v>80</v>
       </c>
       <c r="Z20" s="16"/>
@@ -2859,7 +3087,7 @@
       <c r="M21" s="16"/>
       <c r="N21" s="16"/>
       <c r="O21" s="16"/>
-      <c r="P21" s="19" t="s">
+      <c r="P21" s="18" t="s">
         <v>86</v>
       </c>
       <c r="Q21" s="16"/>
@@ -2986,7 +3214,7 @@
       <c r="B24" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="16" t="s">
         <v>88</v>
       </c>
       <c r="D24" s="16" t="s">
@@ -3067,7 +3295,7 @@
       <c r="G25" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H25" s="20"/>
+      <c r="H25" s="19"/>
       <c r="I25" s="16" t="s">
         <v>28</v>
       </c>
@@ -3131,7 +3359,7 @@
       <c r="G26" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H26" s="20"/>
+      <c r="H26" s="19"/>
       <c r="I26" s="16" t="s">
         <v>28</v>
       </c>
@@ -3174,166 +3402,166 @@
       <c r="AR26" s="16"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22" t="s">
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
-      <c r="P27" s="22"/>
-      <c r="Q27" s="22"/>
-      <c r="R27" s="22"/>
-      <c r="S27" s="22"/>
-      <c r="T27" s="22"/>
-      <c r="U27" s="22"/>
-      <c r="V27" s="22"/>
-      <c r="W27" s="22"/>
-      <c r="X27" s="22"/>
-      <c r="Y27" s="22"/>
-      <c r="Z27" s="22"/>
-      <c r="AA27" s="22"/>
-      <c r="AB27" s="22"/>
-      <c r="AC27" s="22"/>
-      <c r="AD27" s="22"/>
-      <c r="AE27" s="22"/>
-      <c r="AF27" s="22"/>
-      <c r="AG27" s="22"/>
-      <c r="AH27" s="22"/>
-      <c r="AI27" s="22"/>
-      <c r="AJ27" s="22"/>
-      <c r="AK27" s="22"/>
-      <c r="AL27" s="22"/>
-      <c r="AM27" s="22"/>
-      <c r="AN27" s="22"/>
-      <c r="AO27" s="22"/>
-      <c r="AP27" s="22"/>
-      <c r="AQ27" s="22"/>
-      <c r="AR27" s="22"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+      <c r="V27" s="19"/>
+      <c r="W27" s="19"/>
+      <c r="X27" s="19"/>
+      <c r="Y27" s="19"/>
+      <c r="Z27" s="19"/>
+      <c r="AA27" s="19"/>
+      <c r="AB27" s="19"/>
+      <c r="AC27" s="19"/>
+      <c r="AD27" s="19"/>
+      <c r="AE27" s="19"/>
+      <c r="AF27" s="19"/>
+      <c r="AG27" s="19"/>
+      <c r="AH27" s="19"/>
+      <c r="AI27" s="19"/>
+      <c r="AJ27" s="19"/>
+      <c r="AK27" s="19"/>
+      <c r="AL27" s="19"/>
+      <c r="AM27" s="19"/>
+      <c r="AN27" s="19"/>
+      <c r="AO27" s="19"/>
+      <c r="AP27" s="19"/>
+      <c r="AQ27" s="19"/>
+      <c r="AR27" s="19"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22" t="s">
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
-      <c r="Q28" s="22"/>
-      <c r="R28" s="22"/>
-      <c r="S28" s="22"/>
-      <c r="T28" s="22"/>
-      <c r="U28" s="22"/>
-      <c r="V28" s="22"/>
-      <c r="W28" s="22"/>
-      <c r="X28" s="22"/>
-      <c r="Y28" s="22"/>
-      <c r="Z28" s="22"/>
-      <c r="AA28" s="22"/>
-      <c r="AB28" s="22"/>
-      <c r="AC28" s="22"/>
-      <c r="AD28" s="22"/>
-      <c r="AE28" s="22"/>
-      <c r="AF28" s="22"/>
-      <c r="AG28" s="22"/>
-      <c r="AH28" s="22"/>
-      <c r="AI28" s="22"/>
-      <c r="AJ28" s="22"/>
-      <c r="AK28" s="22"/>
-      <c r="AL28" s="22"/>
-      <c r="AM28" s="22"/>
-      <c r="AN28" s="22"/>
-      <c r="AO28" s="22"/>
-      <c r="AP28" s="22"/>
-      <c r="AQ28" s="22"/>
-      <c r="AR28" s="22"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19"/>
+      <c r="V28" s="19"/>
+      <c r="W28" s="19"/>
+      <c r="X28" s="19"/>
+      <c r="Y28" s="19"/>
+      <c r="Z28" s="19"/>
+      <c r="AA28" s="19"/>
+      <c r="AB28" s="19"/>
+      <c r="AC28" s="19"/>
+      <c r="AD28" s="19"/>
+      <c r="AE28" s="19"/>
+      <c r="AF28" s="19"/>
+      <c r="AG28" s="19"/>
+      <c r="AH28" s="19"/>
+      <c r="AI28" s="19"/>
+      <c r="AJ28" s="19"/>
+      <c r="AK28" s="19"/>
+      <c r="AL28" s="19"/>
+      <c r="AM28" s="19"/>
+      <c r="AN28" s="19"/>
+      <c r="AO28" s="19"/>
+      <c r="AP28" s="19"/>
+      <c r="AQ28" s="19"/>
+      <c r="AR28" s="19"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22" t="s">
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="M29" s="22"/>
-      <c r="N29" s="22"/>
-      <c r="O29" s="22"/>
-      <c r="P29" s="22" t="s">
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="Q29" s="22"/>
-      <c r="R29" s="22"/>
-      <c r="S29" s="22"/>
-      <c r="T29" s="22"/>
-      <c r="U29" s="22"/>
-      <c r="V29" s="22"/>
-      <c r="W29" s="22"/>
-      <c r="X29" s="22"/>
-      <c r="Y29" s="22"/>
-      <c r="Z29" s="22"/>
-      <c r="AA29" s="22"/>
-      <c r="AB29" s="22"/>
-      <c r="AC29" s="22"/>
-      <c r="AD29" s="22"/>
-      <c r="AE29" s="22"/>
-      <c r="AF29" s="22"/>
-      <c r="AG29" s="22"/>
-      <c r="AH29" s="22"/>
-      <c r="AI29" s="22"/>
-      <c r="AJ29" s="22"/>
-      <c r="AK29" s="22"/>
-      <c r="AL29" s="22"/>
-      <c r="AM29" s="22"/>
-      <c r="AN29" s="22"/>
-      <c r="AO29" s="22"/>
-      <c r="AP29" s="22"/>
-      <c r="AQ29" s="22"/>
-      <c r="AR29" s="22"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="19"/>
+      <c r="U29" s="19"/>
+      <c r="V29" s="19"/>
+      <c r="W29" s="19"/>
+      <c r="X29" s="19"/>
+      <c r="Y29" s="19"/>
+      <c r="Z29" s="19"/>
+      <c r="AA29" s="19"/>
+      <c r="AB29" s="19"/>
+      <c r="AC29" s="19"/>
+      <c r="AD29" s="19"/>
+      <c r="AE29" s="19"/>
+      <c r="AF29" s="19"/>
+      <c r="AG29" s="19"/>
+      <c r="AH29" s="19"/>
+      <c r="AI29" s="19"/>
+      <c r="AJ29" s="19"/>
+      <c r="AK29" s="19"/>
+      <c r="AL29" s="19"/>
+      <c r="AM29" s="19"/>
+      <c r="AN29" s="19"/>
+      <c r="AO29" s="19"/>
+      <c r="AP29" s="19"/>
+      <c r="AQ29" s="19"/>
+      <c r="AR29" s="19"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="17" t="s">
@@ -3342,8 +3570,8 @@
       <c r="B30" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="18"/>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
@@ -3396,8 +3624,8 @@
       <c r="B31" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="18"/>
       <c r="E31" s="16"/>
       <c r="F31" s="16"/>
       <c r="G31" s="16"/>
@@ -3451,20 +3679,20 @@
       <c r="C32" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="20" t="s">
+      <c r="D32" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E32" s="20" t="s">
+      <c r="E32" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F32" s="20" t="s">
+      <c r="F32" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="G32" s="20" t="s">
+      <c r="G32" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20" t="s">
+      <c r="H32" s="19"/>
+      <c r="I32" s="19" t="s">
         <v>28</v>
       </c>
       <c r="J32" s="16"/>
@@ -3513,7 +3741,7 @@
       <c r="C33" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="D33" s="19"/>
+      <c r="D33" s="18"/>
       <c r="E33" s="16"/>
       <c r="F33" s="16"/>
       <c r="G33" s="16"/>
@@ -3629,7 +3857,7 @@
       <c r="C35" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="D35" s="19"/>
+      <c r="D35" s="18"/>
       <c r="E35" s="16"/>
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
@@ -3683,13 +3911,13 @@
       <c r="A36" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="21" t="s">
         <v>123</v>
       </c>
       <c r="C36" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="D36" s="19"/>
+      <c r="D36" s="18"/>
       <c r="E36" s="16"/>
       <c r="F36" s="16"/>
       <c r="G36" s="16"/>
@@ -3747,7 +3975,7 @@
       <c r="C37" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="D37" s="19"/>
+      <c r="D37" s="18"/>
       <c r="E37" s="16"/>
       <c r="F37" s="16"/>
       <c r="G37" s="16"/>
@@ -3799,7 +4027,7 @@
         <v>131</v>
       </c>
       <c r="C38" s="16"/>
-      <c r="D38" s="19"/>
+      <c r="D38" s="18"/>
       <c r="E38" s="16"/>
       <c r="F38" s="16"/>
       <c r="G38" s="16"/>
@@ -3811,7 +4039,7 @@
       <c r="M38" s="16"/>
       <c r="N38" s="16"/>
       <c r="O38" s="16"/>
-      <c r="P38" s="16" t="s">
+      <c r="P38" s="22" t="s">
         <v>132</v>
       </c>
       <c r="Q38" s="16"/>
@@ -3851,7 +4079,7 @@
         <v>133</v>
       </c>
       <c r="C39" s="16"/>
-      <c r="D39" s="19"/>
+      <c r="D39" s="18"/>
       <c r="E39" s="16"/>
       <c r="F39" s="16"/>
       <c r="G39" s="16"/>
@@ -3863,7 +4091,7 @@
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
       <c r="O39" s="16"/>
-      <c r="P39" s="16" t="s">
+      <c r="P39" s="22" t="s">
         <v>134</v>
       </c>
       <c r="Q39" s="16"/>
@@ -3905,7 +4133,7 @@
       <c r="C40" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="D40" s="19"/>
+      <c r="D40" s="18"/>
       <c r="E40" s="16"/>
       <c r="F40" s="16"/>
       <c r="G40" s="16"/>
@@ -3957,7 +4185,7 @@
         <v>138</v>
       </c>
       <c r="C41" s="16"/>
-      <c r="D41" s="19"/>
+      <c r="D41" s="18"/>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
       <c r="G41" s="16"/>
@@ -4008,10 +4236,10 @@
       <c r="B42" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="C42" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="D42" s="19"/>
+      <c r="D42" s="18"/>
       <c r="E42" s="16"/>
       <c r="F42" s="16"/>
       <c r="G42" s="16"/>
@@ -4065,7 +4293,7 @@
       <c r="C43" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="D43" s="19"/>
+      <c r="D43" s="18"/>
       <c r="E43" s="16"/>
       <c r="F43" s="16"/>
       <c r="G43" s="16"/>
@@ -4116,7 +4344,7 @@
       </c>
       <c r="B44" s="17"/>
       <c r="C44" s="16"/>
-      <c r="D44" s="19"/>
+      <c r="D44" s="18"/>
       <c r="E44" s="16"/>
       <c r="F44" s="16"/>
       <c r="G44" s="16"/>
@@ -4165,7 +4393,7 @@
       <c r="B45" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="C45" s="18" t="s">
+      <c r="C45" s="16" t="s">
         <v>147</v>
       </c>
       <c r="D45" s="16" t="s">
@@ -4191,10 +4419,10 @@
       <c r="L45" s="16"/>
       <c r="M45" s="16"/>
       <c r="N45" s="24" t="b">
-        <f t="shared" ref="N45:N46" si="1">TRUE()</f>
+        <f t="shared" ref="N45:N46" si="0">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="O45" s="18" t="s">
+      <c r="O45" s="16" t="s">
         <v>153</v>
       </c>
       <c r="P45" s="16"/>
@@ -4234,7 +4462,7 @@
       <c r="B46" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="C46" s="18" t="s">
+      <c r="C46" s="16" t="s">
         <v>155</v>
       </c>
       <c r="D46" s="16" t="s">
@@ -4260,10 +4488,10 @@
       <c r="L46" s="16"/>
       <c r="M46" s="16"/>
       <c r="N46" s="24" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O46" s="18" t="s">
+      <c r="O46" s="16" t="s">
         <v>153</v>
       </c>
       <c r="P46" s="16"/>
@@ -4365,58 +4593,58 @@
       <c r="AR47" s="16"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" s="21" t="s">
+      <c r="A48" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B48" s="21" t="s">
+      <c r="B48" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="C48" s="22" t="s">
+      <c r="C48" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="D48" s="22"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="22"/>
-      <c r="G48" s="22"/>
-      <c r="H48" s="22"/>
-      <c r="I48" s="22"/>
-      <c r="J48" s="22"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="19"/>
       <c r="K48" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="L48" s="22"/>
-      <c r="M48" s="22"/>
-      <c r="N48" s="22"/>
-      <c r="O48" s="22"/>
-      <c r="P48" s="22"/>
-      <c r="Q48" s="22"/>
-      <c r="R48" s="22"/>
-      <c r="S48" s="22"/>
-      <c r="T48" s="22"/>
-      <c r="U48" s="22"/>
-      <c r="V48" s="22"/>
-      <c r="W48" s="22"/>
-      <c r="X48" s="22"/>
-      <c r="Y48" s="22"/>
-      <c r="Z48" s="22"/>
-      <c r="AA48" s="22"/>
-      <c r="AB48" s="22"/>
-      <c r="AC48" s="22"/>
-      <c r="AD48" s="22"/>
-      <c r="AE48" s="22"/>
-      <c r="AF48" s="22"/>
-      <c r="AG48" s="22"/>
-      <c r="AH48" s="22"/>
-      <c r="AI48" s="22"/>
-      <c r="AJ48" s="22"/>
-      <c r="AK48" s="22"/>
-      <c r="AL48" s="22"/>
-      <c r="AM48" s="22"/>
-      <c r="AN48" s="22"/>
-      <c r="AO48" s="22"/>
-      <c r="AP48" s="22"/>
-      <c r="AQ48" s="22"/>
-      <c r="AR48" s="22"/>
+      <c r="L48" s="19"/>
+      <c r="M48" s="19"/>
+      <c r="N48" s="19"/>
+      <c r="O48" s="19"/>
+      <c r="P48" s="19"/>
+      <c r="Q48" s="19"/>
+      <c r="R48" s="19"/>
+      <c r="S48" s="19"/>
+      <c r="T48" s="19"/>
+      <c r="U48" s="19"/>
+      <c r="V48" s="19"/>
+      <c r="W48" s="19"/>
+      <c r="X48" s="19"/>
+      <c r="Y48" s="19"/>
+      <c r="Z48" s="19"/>
+      <c r="AA48" s="19"/>
+      <c r="AB48" s="19"/>
+      <c r="AC48" s="19"/>
+      <c r="AD48" s="19"/>
+      <c r="AE48" s="19"/>
+      <c r="AF48" s="19"/>
+      <c r="AG48" s="19"/>
+      <c r="AH48" s="19"/>
+      <c r="AI48" s="19"/>
+      <c r="AJ48" s="19"/>
+      <c r="AK48" s="19"/>
+      <c r="AL48" s="19"/>
+      <c r="AM48" s="19"/>
+      <c r="AN48" s="19"/>
+      <c r="AO48" s="19"/>
+      <c r="AP48" s="19"/>
+      <c r="AQ48" s="19"/>
+      <c r="AR48" s="19"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="17" t="s">
@@ -4444,7 +4672,7 @@
       <c r="I49" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="J49" s="18" t="s">
+      <c r="J49" s="16" t="s">
         <v>47</v>
       </c>
       <c r="K49" s="16" t="s">
@@ -5296,7 +5524,7 @@
       <c r="C64" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="D64" s="19" t="s">
+      <c r="D64" s="18" t="s">
         <v>217</v>
       </c>
       <c r="E64" s="16" t="s">
@@ -5371,7 +5599,7 @@
       <c r="F65" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="G65" s="19" t="s">
+      <c r="G65" s="18" t="s">
         <v>191</v>
       </c>
       <c r="H65" s="16"/>
@@ -5485,7 +5713,7 @@
       <c r="F67" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="G67" s="19" t="s">
+      <c r="G67" s="18" t="s">
         <v>197</v>
       </c>
       <c r="H67" s="16"/>
@@ -5653,7 +5881,7 @@
       <c r="F70" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G70" s="19" t="s">
+      <c r="G70" s="18" t="s">
         <v>28</v>
       </c>
       <c r="H70" s="16"/>
@@ -6879,33 +7107,36 @@
     <row r="1002" ht="15.75" customHeight="1"/>
     <row r="1003" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="landscape" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
-    <pageSetUpPr/>
+    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.14"/>
+    <col customWidth="1" min="1" max="1" width="21.140000000000001"/>
     <col customWidth="1" min="2" max="2" width="14.43"/>
-    <col customWidth="1" min="3" max="3" width="29.0"/>
-    <col customWidth="1" min="4" max="4" width="36.29"/>
-    <col customWidth="1" min="5" max="5" width="27.29"/>
-    <col customWidth="1" min="6" max="7" width="24.71"/>
+    <col customWidth="1" min="3" max="3" width="29"/>
+    <col customWidth="1" min="4" max="4" width="36.289999999999999"/>
+    <col customWidth="1" min="5" max="5" width="27.289999999999999"/>
+    <col customWidth="1" min="6" max="7" width="24.710000000000001"/>
     <col customWidth="1" min="8" max="8" width="7.71"/>
-    <col customWidth="1" min="9" max="9" width="14.29"/>
+    <col customWidth="1" min="9" max="9" width="14.289999999999999"/>
     <col customWidth="1" min="10" max="13" width="7.71"/>
-    <col customWidth="1" min="14" max="26" width="15.14"/>
+    <col customWidth="1" min="14" max="26" width="15.140000000000001"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -6977,7 +7208,7 @@
         <v>232</v>
       </c>
       <c r="H2" s="33"/>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>233</v>
       </c>
       <c r="J2" s="8"/>
@@ -7021,7 +7252,7 @@
         <v>239</v>
       </c>
       <c r="H3" s="33"/>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="19" t="s">
         <v>240</v>
       </c>
       <c r="J3" s="8"/>
@@ -7065,7 +7296,7 @@
         <v>247</v>
       </c>
       <c r="H4" s="33"/>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="19" t="s">
         <v>248</v>
       </c>
       <c r="J4" s="8"/>
@@ -7109,7 +7340,7 @@
         <v>254</v>
       </c>
       <c r="H5" s="33"/>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="19" t="s">
         <v>255</v>
       </c>
       <c r="J5" s="8"/>
@@ -7153,7 +7384,7 @@
         <v>261</v>
       </c>
       <c r="H6" s="33"/>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="19" t="s">
         <v>262</v>
       </c>
       <c r="J6" s="8"/>
@@ -7197,7 +7428,7 @@
         <v>268</v>
       </c>
       <c r="H7" s="33"/>
-      <c r="I7" s="20" t="s">
+      <c r="I7" s="19" t="s">
         <v>269</v>
       </c>
       <c r="J7" s="8"/>
@@ -7241,7 +7472,7 @@
         <v>275</v>
       </c>
       <c r="H8" s="33"/>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="19" t="s">
         <v>276</v>
       </c>
       <c r="J8" s="8"/>
@@ -7277,7 +7508,7 @@
       <c r="F9" s="31"/>
       <c r="G9" s="32"/>
       <c r="H9" s="33"/>
-      <c r="I9" s="20"/>
+      <c r="I9" s="19"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
@@ -7319,7 +7550,7 @@
         <v>286</v>
       </c>
       <c r="H10" s="33"/>
-      <c r="I10" s="20" t="s">
+      <c r="I10" s="19" t="s">
         <v>287</v>
       </c>
       <c r="J10" s="8"/>
@@ -7363,7 +7594,7 @@
         <v>293</v>
       </c>
       <c r="H11" s="33"/>
-      <c r="I11" s="20" t="s">
+      <c r="I11" s="19" t="s">
         <v>294</v>
       </c>
       <c r="J11" s="8"/>
@@ -7407,7 +7638,7 @@
         <v>300</v>
       </c>
       <c r="H12" s="33"/>
-      <c r="I12" s="20" t="s">
+      <c r="I12" s="19" t="s">
         <v>296</v>
       </c>
       <c r="J12" s="8"/>
@@ -7451,7 +7682,7 @@
         <v>303</v>
       </c>
       <c r="H13" s="33"/>
-      <c r="I13" s="20" t="s">
+      <c r="I13" s="19" t="s">
         <v>306</v>
       </c>
       <c r="J13" s="8"/>
@@ -7495,7 +7726,7 @@
         <v>308</v>
       </c>
       <c r="H14" s="33"/>
-      <c r="I14" s="20" t="s">
+      <c r="I14" s="19" t="s">
         <v>233</v>
       </c>
       <c r="J14" s="8"/>
@@ -7539,7 +7770,7 @@
         <v>313</v>
       </c>
       <c r="H15" s="33"/>
-      <c r="I15" s="20" t="s">
+      <c r="I15" s="19" t="s">
         <v>314</v>
       </c>
       <c r="J15" s="8"/>
@@ -7583,7 +7814,7 @@
         <v>320</v>
       </c>
       <c r="H16" s="33"/>
-      <c r="I16" s="20" t="s">
+      <c r="I16" s="19" t="s">
         <v>321</v>
       </c>
       <c r="J16" s="8"/>
@@ -7627,7 +7858,7 @@
         <v>327</v>
       </c>
       <c r="H17" s="33"/>
-      <c r="I17" s="20" t="s">
+      <c r="I17" s="19" t="s">
         <v>328</v>
       </c>
       <c r="J17" s="8"/>
@@ -7671,7 +7902,7 @@
         <v>331</v>
       </c>
       <c r="H18" s="33"/>
-      <c r="I18" s="20" t="s">
+      <c r="I18" s="19" t="s">
         <v>334</v>
       </c>
       <c r="J18" s="8"/>
@@ -7715,7 +7946,7 @@
         <v>339</v>
       </c>
       <c r="H19" s="33"/>
-      <c r="I19" s="20" t="s">
+      <c r="I19" s="19" t="s">
         <v>340</v>
       </c>
       <c r="J19" s="8"/>
@@ -7759,7 +7990,7 @@
         <v>345</v>
       </c>
       <c r="H20" s="33"/>
-      <c r="I20" s="20" t="s">
+      <c r="I20" s="19" t="s">
         <v>346</v>
       </c>
       <c r="J20" s="8"/>
@@ -7803,7 +8034,7 @@
         <v>351</v>
       </c>
       <c r="H21" s="33"/>
-      <c r="I21" s="20" t="s">
+      <c r="I21" s="19" t="s">
         <v>352</v>
       </c>
       <c r="J21" s="8"/>
@@ -7847,7 +8078,7 @@
         <v>217</v>
       </c>
       <c r="H22" s="33"/>
-      <c r="I22" s="20" t="s">
+      <c r="I22" s="19" t="s">
         <v>220</v>
       </c>
       <c r="J22" s="8"/>
@@ -8845,31 +9076,34 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="landscape" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
-    <pageSetUpPr/>
+    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="28.14"/>
-    <col customWidth="1" min="2" max="2" width="12.71"/>
-    <col customWidth="1" min="3" max="3" width="19.0"/>
+    <col customWidth="1" min="1" max="1" width="28.140000000000001"/>
+    <col customWidth="1" min="2" max="2" width="12.710000000000001"/>
+    <col customWidth="1" min="3" max="3" width="19"/>
     <col customWidth="1" min="4" max="4" width="5.71"/>
-    <col customWidth="1" min="5" max="5" width="14.29"/>
-    <col customWidth="1" min="6" max="6" width="34.0"/>
+    <col customWidth="1" min="5" max="5" width="14.289999999999999"/>
+    <col customWidth="1" min="6" max="6" width="34"/>
     <col customWidth="1" min="7" max="14" width="7.71"/>
-    <col customWidth="1" min="15" max="25" width="15.14"/>
+    <col customWidth="1" min="15" max="25" width="15.140000000000001"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -8917,8 +9151,8 @@
         <v>360</v>
       </c>
       <c r="C2" s="40" t="str">
-        <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2021-08-18_00-06</v>
+        <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
+        <v xml:space="preserve">2022-02-25 15-16</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>361</v>
@@ -15614,9 +15848,9 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="landscape" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
6345 - Uplift to enketo-core version 5.18.1 (#7256)
Co-authored-by: Jennifer Q <66472237+latin-panda@users.noreply.github.com>

(cherry picked from commit 2a25f877e0a0d8b37d9387fd294943ed6549d2a9)
</commit_message>
<xml_diff>
--- a/config/covid-19/forms/contact/PLACE_TYPE-create.xlsx
+++ b/config/covid-19/forms/contact/PLACE_TYPE-create.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="survey" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="choices" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="settings" sheetId="3" r:id="rId6"/>
+    <sheet name="survey" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="choices" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="settings" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mjoid+fSX0Qkhf0uQyogBH92gIeJg=="/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="363">
   <si>
     <t>type</t>
   </si>
@@ -98,7 +95,7 @@
     <t>notes</t>
   </si>
   <si>
-    <t>begin group</t>
+    <t xml:space="preserve">begin group</t>
   </si>
   <si>
     <t>inputs</t>
@@ -116,19 +113,19 @@
     <t>contact_id</t>
   </si>
   <si>
-    <t>Contact ID of the logged in user</t>
+    <t xml:space="preserve">Contact ID of the logged in user</t>
   </si>
   <si>
     <t>facility_id</t>
   </si>
   <si>
-    <t>Place ID of the logged in user</t>
-  </si>
-  <si>
-    <t>Name of the logged in user</t>
-  </si>
-  <si>
-    <t>end group</t>
+    <t xml:space="preserve">Place ID of the logged in user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of the logged in user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end group</t>
   </si>
   <si>
     <t>init</t>
@@ -137,28 +134,28 @@
     <t>field-list</t>
   </si>
   <si>
-    <t>select_one contact</t>
+    <t xml:space="preserve">select_one contact</t>
   </si>
   <si>
     <t>create_new_person</t>
   </si>
   <si>
-    <t>Set the primary contact</t>
-  </si>
-  <si>
-    <t>प्राथमिक कॉंटॅक्ट चुनें</t>
-  </si>
-  <si>
-    <t>Ditetapkan Sebagai Kontak Utama</t>
-  </si>
-  <si>
-    <t>Weka mwasiliwa mkuu</t>
-  </si>
-  <si>
-    <t>प्राथमिक सम्पर्क व्यक्ति</t>
-  </si>
-  <si>
-    <t>Contact primaire</t>
+    <t xml:space="preserve">Set the primary contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">प्राथमिक कॉंटॅक्ट चुनें</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ditetapkan Sebagai Kontak Utama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weka mwasiliwa mkuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">प्राथमिक सम्पर्क व्यक्ति</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact primaire</t>
   </si>
   <si>
     <t>yes</t>
@@ -173,19 +170,19 @@
     <t>select_person</t>
   </si>
   <si>
-    <t>Select the primary contact</t>
-  </si>
-  <si>
-    <t>Pilih Kontak Utama</t>
-  </si>
-  <si>
-    <t>Chagua Mwasiliwa mkuu</t>
-  </si>
-  <si>
-    <t>प्राथमिक सम्पर्क व्यक्ति छान्नुहोस्</t>
-  </si>
-  <si>
-    <t>Choisisser le contact primaire</t>
+    <t xml:space="preserve">Select the primary contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pilih Kontak Utama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chagua Mwasiliwa mkuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">प्राथमिक सम्पर्क व्यक्ति छान्नुहोस्</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choisisser le contact primaire</t>
   </si>
   <si>
     <t>selected(${create_new_person},'old_person')</t>
@@ -203,10 +200,10 @@
     <t>contact_name</t>
   </si>
   <si>
-    <t>coalesce(../../contact/name, ../name)</t>
-  </si>
-  <si>
-    <t>select_one translate_name_label</t>
+    <t xml:space="preserve">coalesce(../../contact/name, ../name)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one translate_name_label</t>
   </si>
   <si>
     <t>custom_place_name_label_translator</t>
@@ -230,34 +227,34 @@
     <t>${custom_place_name_label}</t>
   </si>
   <si>
-    <t>selected(${create_new_person},'none') or selected(${is_name_generated}, 'false')  or selected(${is_name_generated}, 'no')</t>
-  </si>
-  <si>
-    <t>Standalone question only if no contact is selected, so show label accordingly</t>
-  </si>
-  <si>
-    <t>select_one place_type</t>
+    <t xml:space="preserve">selected(${create_new_person},'none') or selected(${is_name_generated}, 'false')  or selected(${is_name_generated}, 'no')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standalone question only if no contact is selected, so show label accordingly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one place_type</t>
   </si>
   <si>
     <t>place_type</t>
   </si>
   <si>
-    <t>Enter the name of this place</t>
-  </si>
-  <si>
-    <t>इस स्थान का नाम दर्ज करें</t>
-  </si>
-  <si>
-    <t>Masukkan nama tempat ini</t>
-  </si>
-  <si>
-    <t>Jaza jina la eneo hii</t>
-  </si>
-  <si>
-    <t>यस स्थानको नाम लेख्नुहोस्</t>
-  </si>
-  <si>
-    <t>Nom de l'endroit</t>
+    <t xml:space="preserve">Enter the name of this place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">इस स्थान का नाम दर्ज करें</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masukkan nama tempat ini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jaza jina la eneo hii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">यस स्थानको नाम लेख्नुहोस्</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nom de l'endroit</t>
   </si>
   <si>
     <t>PLACE_TYPE</t>
@@ -269,7 +266,7 @@
     <t>jr:choice-name(${place_type},'${place_type}')</t>
   </si>
   <si>
-    <t>select_one generated_name</t>
+    <t xml:space="preserve">select_one generated_name</t>
   </si>
   <si>
     <t>generated_name</t>
@@ -284,19 +281,19 @@
     <t>contact</t>
   </si>
   <si>
-    <t>New person</t>
-  </si>
-  <si>
-    <t>नया व्यक्ति</t>
-  </si>
-  <si>
-    <t>Orang Baru</t>
-  </si>
-  <si>
-    <t>Mtu Mpya</t>
-  </si>
-  <si>
-    <t>Nouvelle personne</t>
+    <t xml:space="preserve">New person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">नया व्यक्ति</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orang Baru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mtu Mpya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nouvelle personne</t>
   </si>
   <si>
     <t>selected(${create_new_person},'new_person')</t>
@@ -314,7 +311,7 @@
     <t>first_name</t>
   </si>
   <si>
-    <t>First name</t>
+    <t xml:space="preserve">First name</t>
   </si>
   <si>
     <t>last_name</t>
@@ -323,7 +320,7 @@
     <t xml:space="preserve">Last name </t>
   </si>
   <si>
-    <t>concat(${first_name}, ' ', ${last_name})</t>
+    <t xml:space="preserve">concat(${first_name}, ' ', ${last_name})</t>
   </si>
   <si>
     <t>date_of_birth</t>
@@ -353,13 +350,13 @@
     <t>not(selected(../dob_method,'approx'))</t>
   </si>
   <si>
-    <t>floor(decimal-date-time(.)) &lt;= floor(decimal-date-time(today()))</t>
-  </si>
-  <si>
-    <t>Date must be before today</t>
-  </si>
-  <si>
-    <t>Date of Birth</t>
+    <t xml:space="preserve">floor(decimal-date-time(.)) &lt;= floor(decimal-date-time(today()))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date must be before today</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of Birth</t>
   </si>
   <si>
     <t>note</t>
@@ -383,10 +380,10 @@
     <t>Years</t>
   </si>
   <si>
-    <t>. &gt;= 0 and . &lt;= 130</t>
-  </si>
-  <si>
-    <t>Age must be between 0 and 130</t>
+    <t xml:space="preserve">. &gt;= 0 and . &lt;= 130</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age must be between 0 and 130</t>
   </si>
   <si>
     <t>age_months</t>
@@ -395,13 +392,13 @@
     <t>Months</t>
   </si>
   <si>
-    <t>. &gt;= 0 and . &lt;= 11</t>
-  </si>
-  <si>
-    <t>Months must between 0 and 11</t>
-  </si>
-  <si>
-    <t>select_multiple select_dob_method</t>
+    <t xml:space="preserve">. &gt;= 0 and . &lt;= 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Months must between 0 and 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_multiple select_dob_method</t>
   </si>
   <si>
     <t>dob_method</t>
@@ -416,13 +413,13 @@
     <t>ephemeral_months</t>
   </si>
   <si>
-    <t>if(format-date-time(today(),"%m") - ../age_months &lt; 0, format-date-time(today(),"%m") - ../age_months + 12, format-date-time(today(),"%m") - ../age_months)</t>
+    <t xml:space="preserve">if(format-date-time(today(),"%m") - coalesce(../age_months, 0) &lt; 0, format-date-time(today(),"%m") - coalesce(../age_months, 0) + 12, format-date-time(today(),"%m") - coalesce(../age_months, 0))</t>
   </si>
   <si>
     <t>ephemeral_years</t>
   </si>
   <si>
-    <t>if(format-date-time(today(),"%m") - ../age_months &lt; 0, format-date-time(today(),"%Y") - ../age_years - 1, format-date-time(today(),"%Y") -../age_years)</t>
+    <t xml:space="preserve">if(format-date-time(today(),"%m") - coalesce(../age_months, 0) &lt; 0, format-date-time(today(),"%Y") - ../age_years - 1, format-date-time(today(),"%Y") -../age_years)</t>
   </si>
   <si>
     <t>dob_approx</t>
@@ -431,13 +428,13 @@
     <t>DOB</t>
   </si>
   <si>
-    <t>concat(string(${ephemeral_years}),'-',if(${ephemeral_months}&lt;10, concat('0',string(${ephemeral_months})), ${ephemeral_months}),'-',string(format-date-time(today(), "%d")))</t>
+    <t xml:space="preserve">concat(string(${ephemeral_years}),'-',if(${ephemeral_months}&lt;10, concat('0',string(${ephemeral_months})), ${ephemeral_months}),'-',string(format-date-time(today(), "%d")))</t>
   </si>
   <si>
     <t>dob_raw</t>
   </si>
   <si>
-    <t>if(not(selected( ../dob_method,'approx')), 
+    <t xml:space="preserve">if(not(selected( ../dob_method,'approx')), 
 ../dob_calendar,
 ../dob_approx)</t>
   </si>
@@ -445,7 +442,7 @@
     <t>dob_iso</t>
   </si>
   <si>
-    <t>Date of birth</t>
+    <t xml:space="preserve">Date of birth</t>
   </si>
   <si>
     <t>format-date-time(../dob_raw,"%Y-%m-%d")</t>
@@ -454,7 +451,7 @@
     <t>dob_debug</t>
   </si>
   <si>
-    <t>Months: ${ephemeral_months}
+    <t xml:space="preserve">Months: ${ephemeral_months}
 Year: ${ephemeral_years}
 DOB Approx: ${dob_approx}
 DOB Calendar: ${dob_calendar}
@@ -467,49 +464,49 @@
     <t>phone</t>
   </si>
   <si>
-    <t>Phone number</t>
-  </si>
-  <si>
-    <t>फोन नंबर</t>
-  </si>
-  <si>
-    <t>Nomor Telepon</t>
-  </si>
-  <si>
-    <t>Namba ya Simi</t>
-  </si>
-  <si>
-    <t>फाेन नम्बर</t>
+    <t xml:space="preserve">Phone number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">फोन नंबर</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nomor Telepon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namba ya Simi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">फाेन नम्बर</t>
   </si>
   <si>
     <t>Téléphone</t>
   </si>
   <si>
-    <t>Please enter a valid local number, or use the standard international format, which includes a plus sign (+) and country code. For example: +13125551211</t>
+    <t xml:space="preserve">Please enter a valid local number, or use the standard international format, which includes a plus sign (+) and country code. For example: +13125551211</t>
   </si>
   <si>
     <t>phone_alternate</t>
   </si>
   <si>
-    <t>Alternate phone number</t>
-  </si>
-  <si>
-    <t>अन्य फोन नंबर</t>
-  </si>
-  <si>
-    <t>Nomor Telepon Alternatif</t>
+    <t xml:space="preserve">Alternate phone number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">अन्य फोन नंबर</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nomor Telepon Alternatif</t>
   </si>
   <si>
     <t xml:space="preserve">Namba Ya </t>
   </si>
   <si>
-    <t>बैकल्पिक फाेन नम्बर</t>
-  </si>
-  <si>
-    <t>Téléphone alternatif</t>
-  </si>
-  <si>
-    <t>select_one male_female</t>
+    <t xml:space="preserve">बैकल्पिक फाेन नम्बर</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Téléphone alternatif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one male_female</t>
   </si>
   <si>
     <t>sex</t>
@@ -521,7 +518,7 @@
     <t>लिंग</t>
   </si>
   <si>
-    <t>Jenis kelamin</t>
+    <t xml:space="preserve">Jenis kelamin</t>
   </si>
   <si>
     <t>Jinsia</t>
@@ -536,7 +533,7 @@
     <t>Address</t>
   </si>
   <si>
-    <t>select_one roles</t>
+    <t xml:space="preserve">select_one roles</t>
   </si>
   <si>
     <t>role</t>
@@ -551,7 +548,7 @@
     <t>Peran</t>
   </si>
   <si>
-    <t>Namba ya simu Nyingine</t>
+    <t xml:space="preserve">Namba ya simu Nyingine</t>
   </si>
   <si>
     <t>भुमिका</t>
@@ -563,46 +560,46 @@
     <t>role_other</t>
   </si>
   <si>
-    <t>Specify other</t>
-  </si>
-  <si>
-    <t>अन्य का उल्‍लेख करें</t>
-  </si>
-  <si>
-    <t>Tentukan lainnya</t>
-  </si>
-  <si>
-    <t>Fafanua vingine</t>
-  </si>
-  <si>
-    <t>अन्य उल्लेख गर्नुहोस्</t>
+    <t xml:space="preserve">Specify other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">अन्य का उल्‍लेख करें</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tentukan lainnya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fafanua vingine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">अन्य उल्लेख गर्नुहोस्</t>
   </si>
   <si>
     <t>Specifier</t>
   </si>
   <si>
-    <t>selected( ${role},'other')</t>
+    <t xml:space="preserve">selected( ${role},'other')</t>
   </si>
   <si>
     <t>external_id</t>
   </si>
   <si>
-    <t>External ID</t>
-  </si>
-  <si>
-    <t>बाहरी ID</t>
-  </si>
-  <si>
-    <t>Eksternal ID</t>
-  </si>
-  <si>
-    <t>Kitambulisho cha nje</t>
-  </si>
-  <si>
-    <t>बाहिरि ID</t>
-  </si>
-  <si>
-    <t>Identifiant externe</t>
+    <t xml:space="preserve">External ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">बाहरी ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eksternal ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kitambulisho cha nje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">बाहिरि ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifiant externe</t>
   </si>
   <si>
     <t>Notes</t>
@@ -644,28 +641,28 @@
     <t>../../../inputs/user/facility_id</t>
   </si>
   <si>
-    <t>select_one yes_no_generated_name</t>
+    <t xml:space="preserve">select_one yes_no_generated_name</t>
   </si>
   <si>
     <t>is_name_generated</t>
   </si>
   <si>
-    <t>Would you like to name the place after the primary contact: "${generated_name_translation}"?</t>
-  </si>
-  <si>
-    <t>क्या आप इस स्थान को प्राथमिक कॉंटॅक्ट का नाम देना चाहेंगे?: ${generated_name_translation}</t>
-  </si>
-  <si>
-    <t>Apakah Anda ingin nama tempat setelah kontak utama: "${generated_name_translation}"?</t>
-  </si>
-  <si>
-    <t>Je, Ungependa kuita eneo hii kama mwasilishi mkuu wa eneo hii? "${generated_name_translation}"?</t>
-  </si>
-  <si>
-    <t>के तपाइ यस स्थानकाे प्राथमिक सम्पर्क नाम दिन चाहानु हुन्छ?:${generated_name_translation}</t>
-  </si>
-  <si>
-    <t>Voulez-vous nommer l'endroit: "${generated_name_translation}"?</t>
+    <t xml:space="preserve">Would you like to name the place after the primary contact: "${generated_name_translation}"?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">क्या आप इस स्थान को प्राथमिक कॉंटॅक्ट का नाम देना चाहेंगे?: ${generated_name_translation}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apakah Anda ingin nama tempat setelah kontak utama: "${generated_name_translation}"?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je, Ungependa kuita eneo hii kama mwasilishi mkuu wa eneo hii? "${generated_name_translation}"?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">के तपाइ यस स्थानकाे प्राथमिक सम्पर्क नाम दिन चाहानु हुन्छ?:${generated_name_translation}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voulez-vous nommer l'endroit: "${generated_name_translation}"?</t>
   </si>
   <si>
     <t>not(selected(${create_new_person},'none'))</t>
@@ -689,19 +686,19 @@
     <t>Nom</t>
   </si>
   <si>
-    <t>if( ( selected(${is_name_generated}, 'true') or selected(${is_name_generated}, 'yes') ), ${generated_name_translation}, ${custom_place_name})</t>
-  </si>
-  <si>
-    <t>Namba ya nje</t>
-  </si>
-  <si>
-    <t>if(selected(${create_new_person},'none'), "", coalesce(${select_person},"NEW"))</t>
+    <t xml:space="preserve">if( ( selected(${is_name_generated}, 'true') or selected(${is_name_generated}, 'yes') ), ${generated_name_translation}, ${custom_place_name})</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namba ya nje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if(selected(${create_new_person},'none'), "", coalesce(${select_person},"NEW"))</t>
   </si>
   <si>
     <t>geolocation</t>
   </si>
   <si>
-    <t>concat(../../inputs/meta/location/lat, concat(' ', ../../inputs/meta/location/long))</t>
+    <t xml:space="preserve">concat(../../inputs/meta/location/lat, concat(' ', ../../inputs/meta/location/long))</t>
   </si>
   <si>
     <t>list_name</t>
@@ -797,64 +794,64 @@
     <t>new_person</t>
   </si>
   <si>
-    <t>Create a new person</t>
-  </si>
-  <si>
-    <t>एक नया व्यक्ति बनाएं</t>
-  </si>
-  <si>
-    <t>Buat orang baru</t>
-  </si>
-  <si>
-    <t>Ongeza mtumizi mpya</t>
-  </si>
-  <si>
-    <t>एक नया व्यक्ति बनाउनुस</t>
-  </si>
-  <si>
-    <t>Créer une nouvelle personne</t>
+    <t xml:space="preserve">Create a new person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">एक नया व्यक्ति बनाएं</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buat orang baru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ongeza mtumizi mpya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">एक नया व्यक्ति बनाउनुस</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer une nouvelle personne</t>
   </si>
   <si>
     <t>old_person</t>
   </si>
   <si>
-    <t>Select an existing person</t>
-  </si>
-  <si>
-    <t>मौजूदा व्यक्ति चुनें</t>
-  </si>
-  <si>
-    <t>Pilih orang yang ada</t>
-  </si>
-  <si>
-    <t>Chagua mtumizi aliyesajlishwa apo awali</t>
-  </si>
-  <si>
-    <t>व्यक्ति छान्नुहोस्</t>
-  </si>
-  <si>
-    <t>Selectiionner une personne existant</t>
+    <t xml:space="preserve">Select an existing person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">मौजूदा व्यक्ति चुनें</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pilih orang yang ada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chagua mtumizi aliyesajlishwa apo awali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">व्यक्ति छान्नुहोस्</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selectiionner une personne existant</t>
   </si>
   <si>
     <t>none</t>
   </si>
   <si>
-    <t>Skip this step</t>
-  </si>
-  <si>
-    <t>इस स्टेप को छोड़ दें</t>
-  </si>
-  <si>
-    <t>Lewati langkah ini</t>
-  </si>
-  <si>
-    <t>Ruka hatua ii</t>
+    <t xml:space="preserve">Skip this step</t>
+  </si>
+  <si>
+    <t xml:space="preserve">इस स्टेप को छोड़ दें</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lewati langkah ini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruka hatua ii</t>
   </si>
   <si>
     <t xml:space="preserve">एख </t>
   </si>
   <si>
-    <t>Sauter cette section</t>
+    <t xml:space="preserve">Sauter cette section</t>
   </si>
   <si>
     <t>select_dob_method</t>
@@ -863,7 +860,7 @@
     <t>approx</t>
   </si>
   <si>
-    <t>Date of birth unknown</t>
+    <t xml:space="preserve">Date of birth unknown</t>
   </si>
   <si>
     <t>roles</t>
@@ -875,16 +872,16 @@
     <t>CHW</t>
   </si>
   <si>
-    <t>सामुदायिक स्वास्थ्य कर्मी</t>
+    <t xml:space="preserve">सामुदायिक स्वास्थ्य कर्मी</t>
   </si>
   <si>
     <t>Kader</t>
   </si>
   <si>
-    <t>Mhudumu wa afya</t>
-  </si>
-  <si>
-    <t>महिला स्वास्थ्य स्वयम् सेविका</t>
+    <t xml:space="preserve">Mhudumu wa afya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">महिला स्वास्थ्य स्वयम् सेविका</t>
   </si>
   <si>
     <t>ASC</t>
@@ -893,22 +890,22 @@
     <t>chw_supervisor</t>
   </si>
   <si>
-    <t>CHW Supervisor</t>
-  </si>
-  <si>
-    <t>सामुदायिक स्वास्थ्य कर्मी के मैनेजर</t>
-  </si>
-  <si>
-    <t>Kader Pengawas</t>
-  </si>
-  <si>
-    <t>Mkuu wa wahudumu wa afya</t>
-  </si>
-  <si>
-    <t>महिला स्वास्थ्य स्वयम् सेविकाको सुपरभाइजर</t>
-  </si>
-  <si>
-    <t>Superviseur ASC</t>
+    <t xml:space="preserve">CHW Supervisor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">सामुदायिक स्वास्थ्य कर्मी के मैनेजर</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kader Pengawas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mkuu wa wahudumu wa afya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">महिला स्वास्थ्य स्वयम् सेविकाको सुपरभाइजर</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Superviseur ASC</t>
   </si>
   <si>
     <t>patient</t>
@@ -953,28 +950,28 @@
     <t>हो</t>
   </si>
   <si>
-    <t>No, I want to name it manually</t>
-  </si>
-  <si>
-    <t>नहीं, मैं इसे मैन्युअल रूप से नाम देना चाहता हूं</t>
-  </si>
-  <si>
-    <t>Tidak, saya ingin nama itu secara manual</t>
-  </si>
-  <si>
-    <t>Hapana, ningependa kuijaza mwenyewe</t>
-  </si>
-  <si>
-    <t>होइन, म आफैँ नाम दिन चाहन्छु</t>
-  </si>
-  <si>
-    <t>Non, je veux nommer ça manuellement</t>
+    <t xml:space="preserve">No, I want to name it manually</t>
+  </si>
+  <si>
+    <t xml:space="preserve">नहीं, मैं इसे मैन्युअल रूप से नाम देना चाहता हूं</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tidak, saya ingin nama itu secara manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hapana, ningependa kuijaza mwenyewe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">होइन, म आफैँ नाम दिन चाहन्छु</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non, je veux nommer ça manuellement</t>
   </si>
   <si>
     <t>district_hospital</t>
   </si>
   <si>
-    <t>Health Facility</t>
+    <t xml:space="preserve">Health Facility</t>
   </si>
   <si>
     <t>ज़िला</t>
@@ -998,19 +995,19 @@
     <t>Area</t>
   </si>
   <si>
-    <t>स्वास्थ्य केंद्र</t>
-  </si>
-  <si>
-    <t>Fasilitas Kesehatan</t>
-  </si>
-  <si>
-    <t>Kituo cha afya</t>
-  </si>
-  <si>
-    <t>स्वास्थ्य केन्द्र</t>
-  </si>
-  <si>
-    <t>Centre de santé</t>
+    <t xml:space="preserve">स्वास्थ्य केंद्र</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fasilitas Kesehatan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kituo cha afya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">स्वास्थ्य केन्द्र</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centre de santé</t>
   </si>
   <si>
     <t>clinic</t>
@@ -1031,58 +1028,58 @@
     <t>Zone</t>
   </si>
   <si>
-    <t>${contact_name}'s Health Facility</t>
-  </si>
-  <si>
-    <t>${contact_name} का ज़िला</t>
+    <t xml:space="preserve">${contact_name}'s Health Facility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${contact_name} का ज़िला</t>
   </si>
   <si>
     <t xml:space="preserve">Kabupaten ${contact_name} </t>
   </si>
   <si>
-    <t>WIlaya ya  ${contact_name}</t>
+    <t xml:space="preserve">WIlaya ya  ${contact_name}</t>
   </si>
   <si>
     <t xml:space="preserve">${contact_name}को जिल्ला </t>
   </si>
   <si>
-    <t>District de ${contact_name}</t>
-  </si>
-  <si>
-    <t>${contact_name}'s Area</t>
-  </si>
-  <si>
-    <t>${contact_name} का स्वास्थ्य केंद्र</t>
+    <t xml:space="preserve">District de ${contact_name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${contact_name}'s Area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${contact_name} का स्वास्थ्य केंद्र</t>
   </si>
   <si>
     <t xml:space="preserve">Fasilitas Kesehatan ${contact_name} </t>
   </si>
   <si>
-    <t>Kituo cha afya cha  ${contact_name}</t>
-  </si>
-  <si>
-    <t>${contact_name}को स्वास्थ्य केन्द्र</t>
-  </si>
-  <si>
-    <t>Centre de santé de ${contact_name}</t>
-  </si>
-  <si>
-    <t>${contact_name}'s Household</t>
-  </si>
-  <si>
-    <t>${contact_name} का क्षेत्र</t>
+    <t xml:space="preserve">Kituo cha afya cha  ${contact_name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${contact_name}को स्वास्थ्य केन्द्र</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centre de santé de ${contact_name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${contact_name}'s Household</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${contact_name} का क्षेत्र</t>
   </si>
   <si>
     <t xml:space="preserve">Daerah ${contact_name} </t>
   </si>
   <si>
-    <t>Eneo ya  ${contact_name}</t>
-  </si>
-  <si>
-    <t>${contact_name}को क्षेत्र</t>
-  </si>
-  <si>
-    <t>Zone de ${contact_name}</t>
+    <t xml:space="preserve">Eneo ya  ${contact_name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${contact_name}को क्षेत्र</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone de ${contact_name}</t>
   </si>
   <si>
     <t>translate_name_label</t>
@@ -1103,7 +1100,7 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>New PLACE_NAME</t>
+    <t xml:space="preserve">New PLACE_NAME</t>
   </si>
   <si>
     <t>contact:PLACE_TYPE:create</t>
@@ -1118,32 +1115,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <color indexed="64"/>
+      <sz val="11.000000"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b/>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <color indexed="64"/>
+      <sz val="11.000000"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <name val="Calibri"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="11.000000"/>
     </font>
     <font>
-      <sz val="11.0"/>
       <name val="Calibri"/>
+      <sz val="11.000000"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
+      <color indexed="64"/>
+      <sz val="11.000000"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1151,7 +1148,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1209,169 +1206,388 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor indexed="65"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
-    <border/>
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
   <cellXfs count="41">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf fontId="1" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf fontId="1" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="1" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="1" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="1" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf fontId="2" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="2" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf fontId="3" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="3" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="2" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="2" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="2" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="4" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="8" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="9" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf fontId="0" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="10" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="10" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="11" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1428,7 +1644,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1454,7 +1670,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1506,16 +1722,28 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1531,7 +1759,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1561,49 +1789,49 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
-    <pageSetUpPr/>
+    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2.0" ySplit="1.0" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="C1" sqref="C1" pane="topRight"/>
-      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
-      <selection activeCell="C2" sqref="C2" pane="bottomRight"/>
+    <sheetView workbookViewId="0" zoomScale="100">
+      <pane activePane="bottomRight" state="frozen" topLeftCell="C2" xSplit="2" ySplit="1"/>
+      <selection activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="34.0"/>
-    <col customWidth="1" min="2" max="2" width="26.0"/>
-    <col customWidth="1" min="3" max="3" width="47.86"/>
+    <col customWidth="1" min="1" max="1" width="34"/>
+    <col customWidth="1" min="2" max="2" width="26"/>
+    <col customWidth="1" min="3" max="3" width="47.859999999999999"/>
     <col customWidth="1" hidden="1" min="4" max="4" width="33.43"/>
     <col customWidth="1" hidden="1" min="5" max="5" width="27.43"/>
-    <col customWidth="1" hidden="1" min="6" max="6" width="37.29"/>
-    <col customWidth="1" hidden="1" min="7" max="7" width="31.29"/>
-    <col customWidth="1" hidden="1" min="8" max="8" width="8.14"/>
-    <col customWidth="1" hidden="1" min="9" max="9" width="16.71"/>
-    <col customWidth="1" min="10" max="10" width="8.14"/>
+    <col customWidth="1" hidden="1" min="6" max="6" width="37.289999999999999"/>
+    <col customWidth="1" hidden="1" min="7" max="7" width="31.289999999999999"/>
+    <col customWidth="1" hidden="1" min="8" max="8" width="8.1400000000000006"/>
+    <col customWidth="1" hidden="1" min="9" max="9" width="16.710000000000001"/>
+    <col customWidth="1" min="10" max="10" width="8.1400000000000006"/>
     <col customWidth="1" min="11" max="11" width="51.43"/>
-    <col customWidth="1" min="12" max="13" width="10.71"/>
-    <col customWidth="1" min="14" max="14" width="25.29"/>
-    <col customWidth="1" min="15" max="15" width="46.29"/>
-    <col customWidth="1" min="16" max="16" width="68.86"/>
-    <col customWidth="1" min="17" max="17" width="9.43"/>
+    <col customWidth="1" min="12" max="13" width="10.710000000000001"/>
+    <col customWidth="1" min="14" max="14" width="25.289999999999999"/>
+    <col customWidth="1" min="15" max="15" width="46.289999999999999"/>
+    <col customWidth="1" min="16" max="16" width="68.859999999999999"/>
+    <col customWidth="1" min="17" max="17" width="9.4299999999999997"/>
     <col customWidth="1" min="18" max="18" width="33.43"/>
-    <col customWidth="1" min="19" max="19" width="36.29"/>
+    <col customWidth="1" min="19" max="19" width="36.289999999999999"/>
     <col customWidth="1" min="20" max="23" width="13.57"/>
     <col customWidth="1" min="24" max="24" width="7.71"/>
-    <col customWidth="1" min="25" max="25" width="8.71"/>
-    <col customWidth="1" min="26" max="26" width="35.86"/>
+    <col customWidth="1" min="25" max="25" width="8.7100000000000009"/>
+    <col customWidth="1" min="26" max="26" width="35.859999999999999"/>
     <col customWidth="1" min="27" max="36" width="7.71"/>
-    <col customWidth="1" min="37" max="38" width="15.14"/>
-    <col customWidth="1" min="39" max="44" width="17.29"/>
+    <col customWidth="1" min="37" max="38" width="15.140000000000001"/>
+    <col customWidth="1" min="39" max="44" width="17.289999999999999"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -2224,7 +2452,7 @@
       <c r="B11" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="16" t="s">
         <v>41</v>
       </c>
       <c r="D11" s="16" t="s">
@@ -2290,7 +2518,7 @@
       <c r="B12" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="16" t="s">
         <v>51</v>
       </c>
       <c r="D12" s="16" t="s">
@@ -2435,7 +2663,7 @@
       <c r="M14" s="16"/>
       <c r="N14" s="16"/>
       <c r="O14" s="16"/>
-      <c r="P14" s="19" t="s">
+      <c r="P14" s="18" t="s">
         <v>61</v>
       </c>
       <c r="Q14" s="16"/>
@@ -2477,7 +2705,7 @@
       <c r="C15" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="18" t="s">
         <v>28</v>
       </c>
       <c r="E15" s="16" t="s">
@@ -2543,7 +2771,7 @@
         <v>66</v>
       </c>
       <c r="C16" s="16"/>
-      <c r="D16" s="19"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
@@ -2554,8 +2782,8 @@
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19" t="s">
+      <c r="O16" s="18"/>
+      <c r="P16" s="18" t="s">
         <v>67</v>
       </c>
       <c r="Q16" s="16"/>
@@ -2689,7 +2917,7 @@
       <c r="M18" s="16"/>
       <c r="N18" s="16"/>
       <c r="O18" s="16"/>
-      <c r="P18" s="19"/>
+      <c r="P18" s="18"/>
       <c r="Q18" s="16"/>
       <c r="R18" s="16"/>
       <c r="S18" s="16"/>
@@ -2698,7 +2926,7 @@
       <c r="V18" s="16"/>
       <c r="W18" s="16"/>
       <c r="X18" s="16"/>
-      <c r="Y18" s="19" t="s">
+      <c r="Y18" s="18" t="s">
         <v>80</v>
       </c>
       <c r="Z18" s="16"/>
@@ -2741,7 +2969,7 @@
       <c r="M19" s="16"/>
       <c r="N19" s="16"/>
       <c r="O19" s="16"/>
-      <c r="P19" s="19" t="s">
+      <c r="P19" s="18" t="s">
         <v>82</v>
       </c>
       <c r="Q19" s="16"/>
@@ -2816,7 +3044,7 @@
       <c r="V20" s="16"/>
       <c r="W20" s="16"/>
       <c r="X20" s="16"/>
-      <c r="Y20" s="19" t="s">
+      <c r="Y20" s="18" t="s">
         <v>80</v>
       </c>
       <c r="Z20" s="16"/>
@@ -2859,7 +3087,7 @@
       <c r="M21" s="16"/>
       <c r="N21" s="16"/>
       <c r="O21" s="16"/>
-      <c r="P21" s="19" t="s">
+      <c r="P21" s="18" t="s">
         <v>86</v>
       </c>
       <c r="Q21" s="16"/>
@@ -2986,7 +3214,7 @@
       <c r="B24" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="16" t="s">
         <v>88</v>
       </c>
       <c r="D24" s="16" t="s">
@@ -3067,7 +3295,7 @@
       <c r="G25" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H25" s="20"/>
+      <c r="H25" s="19"/>
       <c r="I25" s="16" t="s">
         <v>28</v>
       </c>
@@ -3131,7 +3359,7 @@
       <c r="G26" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H26" s="20"/>
+      <c r="H26" s="19"/>
       <c r="I26" s="16" t="s">
         <v>28</v>
       </c>
@@ -3174,166 +3402,166 @@
       <c r="AR26" s="16"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22" t="s">
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
-      <c r="P27" s="22"/>
-      <c r="Q27" s="22"/>
-      <c r="R27" s="22"/>
-      <c r="S27" s="22"/>
-      <c r="T27" s="22"/>
-      <c r="U27" s="22"/>
-      <c r="V27" s="22"/>
-      <c r="W27" s="22"/>
-      <c r="X27" s="22"/>
-      <c r="Y27" s="22"/>
-      <c r="Z27" s="22"/>
-      <c r="AA27" s="22"/>
-      <c r="AB27" s="22"/>
-      <c r="AC27" s="22"/>
-      <c r="AD27" s="22"/>
-      <c r="AE27" s="22"/>
-      <c r="AF27" s="22"/>
-      <c r="AG27" s="22"/>
-      <c r="AH27" s="22"/>
-      <c r="AI27" s="22"/>
-      <c r="AJ27" s="22"/>
-      <c r="AK27" s="22"/>
-      <c r="AL27" s="22"/>
-      <c r="AM27" s="22"/>
-      <c r="AN27" s="22"/>
-      <c r="AO27" s="22"/>
-      <c r="AP27" s="22"/>
-      <c r="AQ27" s="22"/>
-      <c r="AR27" s="22"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+      <c r="V27" s="19"/>
+      <c r="W27" s="19"/>
+      <c r="X27" s="19"/>
+      <c r="Y27" s="19"/>
+      <c r="Z27" s="19"/>
+      <c r="AA27" s="19"/>
+      <c r="AB27" s="19"/>
+      <c r="AC27" s="19"/>
+      <c r="AD27" s="19"/>
+      <c r="AE27" s="19"/>
+      <c r="AF27" s="19"/>
+      <c r="AG27" s="19"/>
+      <c r="AH27" s="19"/>
+      <c r="AI27" s="19"/>
+      <c r="AJ27" s="19"/>
+      <c r="AK27" s="19"/>
+      <c r="AL27" s="19"/>
+      <c r="AM27" s="19"/>
+      <c r="AN27" s="19"/>
+      <c r="AO27" s="19"/>
+      <c r="AP27" s="19"/>
+      <c r="AQ27" s="19"/>
+      <c r="AR27" s="19"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22" t="s">
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
-      <c r="Q28" s="22"/>
-      <c r="R28" s="22"/>
-      <c r="S28" s="22"/>
-      <c r="T28" s="22"/>
-      <c r="U28" s="22"/>
-      <c r="V28" s="22"/>
-      <c r="W28" s="22"/>
-      <c r="X28" s="22"/>
-      <c r="Y28" s="22"/>
-      <c r="Z28" s="22"/>
-      <c r="AA28" s="22"/>
-      <c r="AB28" s="22"/>
-      <c r="AC28" s="22"/>
-      <c r="AD28" s="22"/>
-      <c r="AE28" s="22"/>
-      <c r="AF28" s="22"/>
-      <c r="AG28" s="22"/>
-      <c r="AH28" s="22"/>
-      <c r="AI28" s="22"/>
-      <c r="AJ28" s="22"/>
-      <c r="AK28" s="22"/>
-      <c r="AL28" s="22"/>
-      <c r="AM28" s="22"/>
-      <c r="AN28" s="22"/>
-      <c r="AO28" s="22"/>
-      <c r="AP28" s="22"/>
-      <c r="AQ28" s="22"/>
-      <c r="AR28" s="22"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19"/>
+      <c r="V28" s="19"/>
+      <c r="W28" s="19"/>
+      <c r="X28" s="19"/>
+      <c r="Y28" s="19"/>
+      <c r="Z28" s="19"/>
+      <c r="AA28" s="19"/>
+      <c r="AB28" s="19"/>
+      <c r="AC28" s="19"/>
+      <c r="AD28" s="19"/>
+      <c r="AE28" s="19"/>
+      <c r="AF28" s="19"/>
+      <c r="AG28" s="19"/>
+      <c r="AH28" s="19"/>
+      <c r="AI28" s="19"/>
+      <c r="AJ28" s="19"/>
+      <c r="AK28" s="19"/>
+      <c r="AL28" s="19"/>
+      <c r="AM28" s="19"/>
+      <c r="AN28" s="19"/>
+      <c r="AO28" s="19"/>
+      <c r="AP28" s="19"/>
+      <c r="AQ28" s="19"/>
+      <c r="AR28" s="19"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22" t="s">
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="M29" s="22"/>
-      <c r="N29" s="22"/>
-      <c r="O29" s="22"/>
-      <c r="P29" s="22" t="s">
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="Q29" s="22"/>
-      <c r="R29" s="22"/>
-      <c r="S29" s="22"/>
-      <c r="T29" s="22"/>
-      <c r="U29" s="22"/>
-      <c r="V29" s="22"/>
-      <c r="W29" s="22"/>
-      <c r="X29" s="22"/>
-      <c r="Y29" s="22"/>
-      <c r="Z29" s="22"/>
-      <c r="AA29" s="22"/>
-      <c r="AB29" s="22"/>
-      <c r="AC29" s="22"/>
-      <c r="AD29" s="22"/>
-      <c r="AE29" s="22"/>
-      <c r="AF29" s="22"/>
-      <c r="AG29" s="22"/>
-      <c r="AH29" s="22"/>
-      <c r="AI29" s="22"/>
-      <c r="AJ29" s="22"/>
-      <c r="AK29" s="22"/>
-      <c r="AL29" s="22"/>
-      <c r="AM29" s="22"/>
-      <c r="AN29" s="22"/>
-      <c r="AO29" s="22"/>
-      <c r="AP29" s="22"/>
-      <c r="AQ29" s="22"/>
-      <c r="AR29" s="22"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="19"/>
+      <c r="U29" s="19"/>
+      <c r="V29" s="19"/>
+      <c r="W29" s="19"/>
+      <c r="X29" s="19"/>
+      <c r="Y29" s="19"/>
+      <c r="Z29" s="19"/>
+      <c r="AA29" s="19"/>
+      <c r="AB29" s="19"/>
+      <c r="AC29" s="19"/>
+      <c r="AD29" s="19"/>
+      <c r="AE29" s="19"/>
+      <c r="AF29" s="19"/>
+      <c r="AG29" s="19"/>
+      <c r="AH29" s="19"/>
+      <c r="AI29" s="19"/>
+      <c r="AJ29" s="19"/>
+      <c r="AK29" s="19"/>
+      <c r="AL29" s="19"/>
+      <c r="AM29" s="19"/>
+      <c r="AN29" s="19"/>
+      <c r="AO29" s="19"/>
+      <c r="AP29" s="19"/>
+      <c r="AQ29" s="19"/>
+      <c r="AR29" s="19"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="17" t="s">
@@ -3342,8 +3570,8 @@
       <c r="B30" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="18"/>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
@@ -3396,8 +3624,8 @@
       <c r="B31" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="18"/>
       <c r="E31" s="16"/>
       <c r="F31" s="16"/>
       <c r="G31" s="16"/>
@@ -3451,20 +3679,20 @@
       <c r="C32" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="20" t="s">
+      <c r="D32" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E32" s="20" t="s">
+      <c r="E32" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F32" s="20" t="s">
+      <c r="F32" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="G32" s="20" t="s">
+      <c r="G32" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20" t="s">
+      <c r="H32" s="19"/>
+      <c r="I32" s="19" t="s">
         <v>28</v>
       </c>
       <c r="J32" s="16"/>
@@ -3513,7 +3741,7 @@
       <c r="C33" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="D33" s="19"/>
+      <c r="D33" s="18"/>
       <c r="E33" s="16"/>
       <c r="F33" s="16"/>
       <c r="G33" s="16"/>
@@ -3629,7 +3857,7 @@
       <c r="C35" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="D35" s="19"/>
+      <c r="D35" s="18"/>
       <c r="E35" s="16"/>
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
@@ -3683,13 +3911,13 @@
       <c r="A36" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="21" t="s">
         <v>123</v>
       </c>
       <c r="C36" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="D36" s="19"/>
+      <c r="D36" s="18"/>
       <c r="E36" s="16"/>
       <c r="F36" s="16"/>
       <c r="G36" s="16"/>
@@ -3747,7 +3975,7 @@
       <c r="C37" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="D37" s="19"/>
+      <c r="D37" s="18"/>
       <c r="E37" s="16"/>
       <c r="F37" s="16"/>
       <c r="G37" s="16"/>
@@ -3799,7 +4027,7 @@
         <v>131</v>
       </c>
       <c r="C38" s="16"/>
-      <c r="D38" s="19"/>
+      <c r="D38" s="18"/>
       <c r="E38" s="16"/>
       <c r="F38" s="16"/>
       <c r="G38" s="16"/>
@@ -3811,7 +4039,7 @@
       <c r="M38" s="16"/>
       <c r="N38" s="16"/>
       <c r="O38" s="16"/>
-      <c r="P38" s="16" t="s">
+      <c r="P38" s="22" t="s">
         <v>132</v>
       </c>
       <c r="Q38" s="16"/>
@@ -3851,7 +4079,7 @@
         <v>133</v>
       </c>
       <c r="C39" s="16"/>
-      <c r="D39" s="19"/>
+      <c r="D39" s="18"/>
       <c r="E39" s="16"/>
       <c r="F39" s="16"/>
       <c r="G39" s="16"/>
@@ -3863,7 +4091,7 @@
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
       <c r="O39" s="16"/>
-      <c r="P39" s="16" t="s">
+      <c r="P39" s="22" t="s">
         <v>134</v>
       </c>
       <c r="Q39" s="16"/>
@@ -3905,7 +4133,7 @@
       <c r="C40" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="D40" s="19"/>
+      <c r="D40" s="18"/>
       <c r="E40" s="16"/>
       <c r="F40" s="16"/>
       <c r="G40" s="16"/>
@@ -3957,7 +4185,7 @@
         <v>138</v>
       </c>
       <c r="C41" s="16"/>
-      <c r="D41" s="19"/>
+      <c r="D41" s="18"/>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
       <c r="G41" s="16"/>
@@ -4008,10 +4236,10 @@
       <c r="B42" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="C42" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="D42" s="19"/>
+      <c r="D42" s="18"/>
       <c r="E42" s="16"/>
       <c r="F42" s="16"/>
       <c r="G42" s="16"/>
@@ -4065,7 +4293,7 @@
       <c r="C43" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="D43" s="19"/>
+      <c r="D43" s="18"/>
       <c r="E43" s="16"/>
       <c r="F43" s="16"/>
       <c r="G43" s="16"/>
@@ -4116,7 +4344,7 @@
       </c>
       <c r="B44" s="17"/>
       <c r="C44" s="16"/>
-      <c r="D44" s="19"/>
+      <c r="D44" s="18"/>
       <c r="E44" s="16"/>
       <c r="F44" s="16"/>
       <c r="G44" s="16"/>
@@ -4165,7 +4393,7 @@
       <c r="B45" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="C45" s="18" t="s">
+      <c r="C45" s="16" t="s">
         <v>147</v>
       </c>
       <c r="D45" s="16" t="s">
@@ -4191,10 +4419,10 @@
       <c r="L45" s="16"/>
       <c r="M45" s="16"/>
       <c r="N45" s="24" t="b">
-        <f t="shared" ref="N45:N46" si="1">TRUE()</f>
+        <f t="shared" ref="N45:N46" si="0">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="O45" s="18" t="s">
+      <c r="O45" s="16" t="s">
         <v>153</v>
       </c>
       <c r="P45" s="16"/>
@@ -4234,7 +4462,7 @@
       <c r="B46" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="C46" s="18" t="s">
+      <c r="C46" s="16" t="s">
         <v>155</v>
       </c>
       <c r="D46" s="16" t="s">
@@ -4260,10 +4488,10 @@
       <c r="L46" s="16"/>
       <c r="M46" s="16"/>
       <c r="N46" s="24" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O46" s="18" t="s">
+      <c r="O46" s="16" t="s">
         <v>153</v>
       </c>
       <c r="P46" s="16"/>
@@ -4365,58 +4593,58 @@
       <c r="AR47" s="16"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" s="21" t="s">
+      <c r="A48" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B48" s="21" t="s">
+      <c r="B48" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="C48" s="22" t="s">
+      <c r="C48" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="D48" s="22"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="22"/>
-      <c r="G48" s="22"/>
-      <c r="H48" s="22"/>
-      <c r="I48" s="22"/>
-      <c r="J48" s="22"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="19"/>
       <c r="K48" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="L48" s="22"/>
-      <c r="M48" s="22"/>
-      <c r="N48" s="22"/>
-      <c r="O48" s="22"/>
-      <c r="P48" s="22"/>
-      <c r="Q48" s="22"/>
-      <c r="R48" s="22"/>
-      <c r="S48" s="22"/>
-      <c r="T48" s="22"/>
-      <c r="U48" s="22"/>
-      <c r="V48" s="22"/>
-      <c r="W48" s="22"/>
-      <c r="X48" s="22"/>
-      <c r="Y48" s="22"/>
-      <c r="Z48" s="22"/>
-      <c r="AA48" s="22"/>
-      <c r="AB48" s="22"/>
-      <c r="AC48" s="22"/>
-      <c r="AD48" s="22"/>
-      <c r="AE48" s="22"/>
-      <c r="AF48" s="22"/>
-      <c r="AG48" s="22"/>
-      <c r="AH48" s="22"/>
-      <c r="AI48" s="22"/>
-      <c r="AJ48" s="22"/>
-      <c r="AK48" s="22"/>
-      <c r="AL48" s="22"/>
-      <c r="AM48" s="22"/>
-      <c r="AN48" s="22"/>
-      <c r="AO48" s="22"/>
-      <c r="AP48" s="22"/>
-      <c r="AQ48" s="22"/>
-      <c r="AR48" s="22"/>
+      <c r="L48" s="19"/>
+      <c r="M48" s="19"/>
+      <c r="N48" s="19"/>
+      <c r="O48" s="19"/>
+      <c r="P48" s="19"/>
+      <c r="Q48" s="19"/>
+      <c r="R48" s="19"/>
+      <c r="S48" s="19"/>
+      <c r="T48" s="19"/>
+      <c r="U48" s="19"/>
+      <c r="V48" s="19"/>
+      <c r="W48" s="19"/>
+      <c r="X48" s="19"/>
+      <c r="Y48" s="19"/>
+      <c r="Z48" s="19"/>
+      <c r="AA48" s="19"/>
+      <c r="AB48" s="19"/>
+      <c r="AC48" s="19"/>
+      <c r="AD48" s="19"/>
+      <c r="AE48" s="19"/>
+      <c r="AF48" s="19"/>
+      <c r="AG48" s="19"/>
+      <c r="AH48" s="19"/>
+      <c r="AI48" s="19"/>
+      <c r="AJ48" s="19"/>
+      <c r="AK48" s="19"/>
+      <c r="AL48" s="19"/>
+      <c r="AM48" s="19"/>
+      <c r="AN48" s="19"/>
+      <c r="AO48" s="19"/>
+      <c r="AP48" s="19"/>
+      <c r="AQ48" s="19"/>
+      <c r="AR48" s="19"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="17" t="s">
@@ -4444,7 +4672,7 @@
       <c r="I49" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="J49" s="18" t="s">
+      <c r="J49" s="16" t="s">
         <v>47</v>
       </c>
       <c r="K49" s="16" t="s">
@@ -5296,7 +5524,7 @@
       <c r="C64" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="D64" s="19" t="s">
+      <c r="D64" s="18" t="s">
         <v>217</v>
       </c>
       <c r="E64" s="16" t="s">
@@ -5371,7 +5599,7 @@
       <c r="F65" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="G65" s="19" t="s">
+      <c r="G65" s="18" t="s">
         <v>191</v>
       </c>
       <c r="H65" s="16"/>
@@ -5485,7 +5713,7 @@
       <c r="F67" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="G67" s="19" t="s">
+      <c r="G67" s="18" t="s">
         <v>197</v>
       </c>
       <c r="H67" s="16"/>
@@ -5653,7 +5881,7 @@
       <c r="F70" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G70" s="19" t="s">
+      <c r="G70" s="18" t="s">
         <v>28</v>
       </c>
       <c r="H70" s="16"/>
@@ -6879,33 +7107,36 @@
     <row r="1002" ht="15.75" customHeight="1"/>
     <row r="1003" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="landscape" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
-    <pageSetUpPr/>
+    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.14"/>
+    <col customWidth="1" min="1" max="1" width="21.140000000000001"/>
     <col customWidth="1" min="2" max="2" width="14.43"/>
-    <col customWidth="1" min="3" max="3" width="29.0"/>
-    <col customWidth="1" min="4" max="4" width="36.29"/>
-    <col customWidth="1" min="5" max="5" width="27.29"/>
-    <col customWidth="1" min="6" max="7" width="24.71"/>
+    <col customWidth="1" min="3" max="3" width="29"/>
+    <col customWidth="1" min="4" max="4" width="36.289999999999999"/>
+    <col customWidth="1" min="5" max="5" width="27.289999999999999"/>
+    <col customWidth="1" min="6" max="7" width="24.710000000000001"/>
     <col customWidth="1" min="8" max="8" width="7.71"/>
-    <col customWidth="1" min="9" max="9" width="14.29"/>
+    <col customWidth="1" min="9" max="9" width="14.289999999999999"/>
     <col customWidth="1" min="10" max="13" width="7.71"/>
-    <col customWidth="1" min="14" max="26" width="15.14"/>
+    <col customWidth="1" min="14" max="26" width="15.140000000000001"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -6977,7 +7208,7 @@
         <v>232</v>
       </c>
       <c r="H2" s="33"/>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>233</v>
       </c>
       <c r="J2" s="8"/>
@@ -7021,7 +7252,7 @@
         <v>239</v>
       </c>
       <c r="H3" s="33"/>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="19" t="s">
         <v>240</v>
       </c>
       <c r="J3" s="8"/>
@@ -7065,7 +7296,7 @@
         <v>247</v>
       </c>
       <c r="H4" s="33"/>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="19" t="s">
         <v>248</v>
       </c>
       <c r="J4" s="8"/>
@@ -7109,7 +7340,7 @@
         <v>254</v>
       </c>
       <c r="H5" s="33"/>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="19" t="s">
         <v>255</v>
       </c>
       <c r="J5" s="8"/>
@@ -7153,7 +7384,7 @@
         <v>261</v>
       </c>
       <c r="H6" s="33"/>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="19" t="s">
         <v>262</v>
       </c>
       <c r="J6" s="8"/>
@@ -7197,7 +7428,7 @@
         <v>268</v>
       </c>
       <c r="H7" s="33"/>
-      <c r="I7" s="20" t="s">
+      <c r="I7" s="19" t="s">
         <v>269</v>
       </c>
       <c r="J7" s="8"/>
@@ -7241,7 +7472,7 @@
         <v>275</v>
       </c>
       <c r="H8" s="33"/>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="19" t="s">
         <v>276</v>
       </c>
       <c r="J8" s="8"/>
@@ -7277,7 +7508,7 @@
       <c r="F9" s="31"/>
       <c r="G9" s="32"/>
       <c r="H9" s="33"/>
-      <c r="I9" s="20"/>
+      <c r="I9" s="19"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
@@ -7319,7 +7550,7 @@
         <v>286</v>
       </c>
       <c r="H10" s="33"/>
-      <c r="I10" s="20" t="s">
+      <c r="I10" s="19" t="s">
         <v>287</v>
       </c>
       <c r="J10" s="8"/>
@@ -7363,7 +7594,7 @@
         <v>293</v>
       </c>
       <c r="H11" s="33"/>
-      <c r="I11" s="20" t="s">
+      <c r="I11" s="19" t="s">
         <v>294</v>
       </c>
       <c r="J11" s="8"/>
@@ -7407,7 +7638,7 @@
         <v>300</v>
       </c>
       <c r="H12" s="33"/>
-      <c r="I12" s="20" t="s">
+      <c r="I12" s="19" t="s">
         <v>296</v>
       </c>
       <c r="J12" s="8"/>
@@ -7451,7 +7682,7 @@
         <v>303</v>
       </c>
       <c r="H13" s="33"/>
-      <c r="I13" s="20" t="s">
+      <c r="I13" s="19" t="s">
         <v>306</v>
       </c>
       <c r="J13" s="8"/>
@@ -7495,7 +7726,7 @@
         <v>308</v>
       </c>
       <c r="H14" s="33"/>
-      <c r="I14" s="20" t="s">
+      <c r="I14" s="19" t="s">
         <v>233</v>
       </c>
       <c r="J14" s="8"/>
@@ -7539,7 +7770,7 @@
         <v>313</v>
       </c>
       <c r="H15" s="33"/>
-      <c r="I15" s="20" t="s">
+      <c r="I15" s="19" t="s">
         <v>314</v>
       </c>
       <c r="J15" s="8"/>
@@ -7583,7 +7814,7 @@
         <v>320</v>
       </c>
       <c r="H16" s="33"/>
-      <c r="I16" s="20" t="s">
+      <c r="I16" s="19" t="s">
         <v>321</v>
       </c>
       <c r="J16" s="8"/>
@@ -7627,7 +7858,7 @@
         <v>327</v>
       </c>
       <c r="H17" s="33"/>
-      <c r="I17" s="20" t="s">
+      <c r="I17" s="19" t="s">
         <v>328</v>
       </c>
       <c r="J17" s="8"/>
@@ -7671,7 +7902,7 @@
         <v>331</v>
       </c>
       <c r="H18" s="33"/>
-      <c r="I18" s="20" t="s">
+      <c r="I18" s="19" t="s">
         <v>334</v>
       </c>
       <c r="J18" s="8"/>
@@ -7715,7 +7946,7 @@
         <v>339</v>
       </c>
       <c r="H19" s="33"/>
-      <c r="I19" s="20" t="s">
+      <c r="I19" s="19" t="s">
         <v>340</v>
       </c>
       <c r="J19" s="8"/>
@@ -7759,7 +7990,7 @@
         <v>345</v>
       </c>
       <c r="H20" s="33"/>
-      <c r="I20" s="20" t="s">
+      <c r="I20" s="19" t="s">
         <v>346</v>
       </c>
       <c r="J20" s="8"/>
@@ -7803,7 +8034,7 @@
         <v>351</v>
       </c>
       <c r="H21" s="33"/>
-      <c r="I21" s="20" t="s">
+      <c r="I21" s="19" t="s">
         <v>352</v>
       </c>
       <c r="J21" s="8"/>
@@ -7847,7 +8078,7 @@
         <v>217</v>
       </c>
       <c r="H22" s="33"/>
-      <c r="I22" s="20" t="s">
+      <c r="I22" s="19" t="s">
         <v>220</v>
       </c>
       <c r="J22" s="8"/>
@@ -8845,31 +9076,34 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="landscape" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
-    <pageSetUpPr/>
+    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="28.14"/>
-    <col customWidth="1" min="2" max="2" width="12.71"/>
-    <col customWidth="1" min="3" max="3" width="19.0"/>
+    <col customWidth="1" min="1" max="1" width="28.140000000000001"/>
+    <col customWidth="1" min="2" max="2" width="12.710000000000001"/>
+    <col customWidth="1" min="3" max="3" width="19"/>
     <col customWidth="1" min="4" max="4" width="5.71"/>
-    <col customWidth="1" min="5" max="5" width="14.29"/>
-    <col customWidth="1" min="6" max="6" width="34.0"/>
+    <col customWidth="1" min="5" max="5" width="14.289999999999999"/>
+    <col customWidth="1" min="6" max="6" width="34"/>
     <col customWidth="1" min="7" max="14" width="7.71"/>
-    <col customWidth="1" min="15" max="25" width="15.14"/>
+    <col customWidth="1" min="15" max="25" width="15.140000000000001"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -8917,8 +9151,8 @@
         <v>360</v>
       </c>
       <c r="C2" s="40" t="str">
-        <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2021-08-18_00-06</v>
+        <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
+        <v xml:space="preserve">2022-02-25 15-16</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>361</v>
@@ -15614,9 +15848,9 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="landscape" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>